<commit_message>
Update email process with image attachment
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-4230" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="-28920" yWindow="-3780" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <externalReference r:id="rId5"/>
     <externalReference r:id="rId6"/>
   </externalReferences>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -1988,31 +1988,7 @@
     </xf>
     <xf numFmtId="49" fontId="10" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2036,6 +2012,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -2130,6 +2130,1133 @@
     <dxf>
       <fill>
         <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
           <bgColor theme="5"/>
         </patternFill>
       </fill>
@@ -2362,1133 +3489,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5014,7 +5014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
@@ -5309,8 +5309,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L370"/>
   <sheetViews>
-    <sheetView topLeftCell="D345" workbookViewId="0">
-      <selection activeCell="G370" sqref="G370"/>
+    <sheetView tabSelected="1" topLeftCell="F345" workbookViewId="0">
+      <selection activeCell="I368" sqref="I368"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,16 +5367,16 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
-      <c r="C2" s="115" t="s">
+      <c r="C2" s="131" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="115"/>
-      <c r="E2" s="115"/>
-      <c r="F2" s="115"/>
-      <c r="G2" s="115"/>
-      <c r="H2" s="115"/>
-      <c r="I2" s="115"/>
-      <c r="J2" s="115"/>
+      <c r="D2" s="131"/>
+      <c r="E2" s="131"/>
+      <c r="F2" s="131"/>
+      <c r="G2" s="131"/>
+      <c r="H2" s="131"/>
+      <c r="I2" s="131"/>
+      <c r="J2" s="131"/>
       <c r="K2" s="32"/>
       <c r="L2" s="33"/>
     </row>
@@ -6486,16 +6486,16 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="32"/>
-      <c r="C39" s="115" t="s">
+      <c r="C39" s="131" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="115"/>
-      <c r="E39" s="115"/>
-      <c r="F39" s="115"/>
-      <c r="G39" s="115"/>
-      <c r="H39" s="115"/>
-      <c r="I39" s="115"/>
-      <c r="J39" s="115"/>
+      <c r="D39" s="131"/>
+      <c r="E39" s="131"/>
+      <c r="F39" s="131"/>
+      <c r="G39" s="131"/>
+      <c r="H39" s="131"/>
+      <c r="I39" s="131"/>
+      <c r="J39" s="131"/>
       <c r="K39" s="32"/>
       <c r="L39" s="33"/>
     </row>
@@ -7671,16 +7671,16 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="31"/>
       <c r="B79" s="32"/>
-      <c r="C79" s="115" t="s">
+      <c r="C79" s="131" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="115"/>
-      <c r="E79" s="115"/>
-      <c r="F79" s="115"/>
-      <c r="G79" s="115"/>
-      <c r="H79" s="115"/>
-      <c r="I79" s="115"/>
-      <c r="J79" s="115"/>
+      <c r="D79" s="131"/>
+      <c r="E79" s="131"/>
+      <c r="F79" s="131"/>
+      <c r="G79" s="131"/>
+      <c r="H79" s="131"/>
+      <c r="I79" s="131"/>
+      <c r="J79" s="131"/>
       <c r="K79" s="32"/>
       <c r="L79" s="33"/>
     </row>
@@ -8955,16 +8955,16 @@
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="31"/>
       <c r="B124" s="32"/>
-      <c r="C124" s="115" t="s">
+      <c r="C124" s="131" t="s">
         <v>198</v>
       </c>
-      <c r="D124" s="115"/>
-      <c r="E124" s="115"/>
-      <c r="F124" s="115"/>
-      <c r="G124" s="115"/>
-      <c r="H124" s="115"/>
-      <c r="I124" s="115"/>
-      <c r="J124" s="115"/>
+      <c r="D124" s="131"/>
+      <c r="E124" s="131"/>
+      <c r="F124" s="131"/>
+      <c r="G124" s="131"/>
+      <c r="H124" s="131"/>
+      <c r="I124" s="131"/>
+      <c r="J124" s="131"/>
       <c r="K124" s="32"/>
       <c r="L124" s="33"/>
     </row>
@@ -10221,11 +10221,11 @@
       </c>
     </row>
     <row r="167" spans="1:12" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="116" t="s">
+      <c r="B167" s="132" t="s">
         <v>206</v>
       </c>
-      <c r="C167" s="116"/>
-      <c r="D167" s="116"/>
+      <c r="C167" s="132"/>
+      <c r="D167" s="132"/>
       <c r="H167" s="78"/>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -10704,11 +10704,11 @@
       <c r="J183" s="18"/>
     </row>
     <row r="184" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="117" t="s">
+      <c r="B184" s="126" t="s">
         <v>211</v>
       </c>
-      <c r="C184" s="117"/>
-      <c r="D184" s="117"/>
+      <c r="C184" s="126"/>
+      <c r="D184" s="126"/>
       <c r="H184" s="86"/>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
@@ -11009,11 +11009,11 @@
       </c>
     </row>
     <row r="198" spans="1:12" s="90" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B198" s="119" t="s">
+      <c r="B198" s="128" t="s">
         <v>202</v>
       </c>
-      <c r="C198" s="119"/>
-      <c r="D198" s="119"/>
+      <c r="C198" s="128"/>
+      <c r="D198" s="128"/>
       <c r="H198" s="91"/>
     </row>
     <row r="199" spans="1:12" s="114" customFormat="1" x14ac:dyDescent="0.25">
@@ -11539,11 +11539,11 @@
       </c>
     </row>
     <row r="217" spans="1:12" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B217" s="120" t="s">
+      <c r="B217" s="129" t="s">
         <v>203</v>
       </c>
-      <c r="C217" s="120"/>
-      <c r="D217" s="120"/>
+      <c r="C217" s="129"/>
+      <c r="D217" s="129"/>
       <c r="H217" s="78"/>
     </row>
     <row r="218" spans="1:12" s="98" customFormat="1" x14ac:dyDescent="0.25">
@@ -12527,11 +12527,11 @@
       </c>
     </row>
     <row r="251" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B251" s="121" t="s">
+      <c r="B251" s="130" t="s">
         <v>204</v>
       </c>
-      <c r="C251" s="121"/>
-      <c r="D251" s="121"/>
+      <c r="C251" s="130"/>
+      <c r="D251" s="130"/>
       <c r="H251" s="86"/>
     </row>
     <row r="252" spans="1:12" x14ac:dyDescent="0.25">
@@ -12881,11 +12881,11 @@
       </c>
     </row>
     <row r="264" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B264" s="121" t="s">
+      <c r="B264" s="130" t="s">
         <v>205</v>
       </c>
-      <c r="C264" s="121"/>
-      <c r="D264" s="121"/>
+      <c r="C264" s="130"/>
+      <c r="D264" s="130"/>
       <c r="H264" s="86"/>
     </row>
     <row r="265" spans="1:12" x14ac:dyDescent="0.25">
@@ -13547,11 +13547,11 @@
       </c>
     </row>
     <row r="288" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="117" t="s">
+      <c r="B288" s="126" t="s">
         <v>415</v>
       </c>
-      <c r="C288" s="117"/>
-      <c r="D288" s="117"/>
+      <c r="C288" s="126"/>
+      <c r="D288" s="126"/>
       <c r="H288" s="86"/>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -13830,11 +13830,11 @@
       </c>
     </row>
     <row r="298" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="118" t="s">
+      <c r="B298" s="127" t="s">
         <v>414</v>
       </c>
-      <c r="C298" s="118"/>
-      <c r="D298" s="118"/>
+      <c r="C298" s="127"/>
+      <c r="D298" s="127"/>
       <c r="H298" s="86"/>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -14081,20 +14081,20 @@
       </c>
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A307" s="122"/>
-      <c r="B307" s="123" t="s">
+      <c r="A307" s="115"/>
+      <c r="B307" s="125" t="s">
         <v>427</v>
       </c>
-      <c r="C307" s="123"/>
-      <c r="D307" s="123"/>
-      <c r="E307" s="123"/>
-      <c r="F307" s="122"/>
-      <c r="G307" s="122"/>
-      <c r="H307" s="124"/>
-      <c r="I307" s="122"/>
-      <c r="J307" s="122"/>
-      <c r="K307" s="122"/>
-      <c r="L307" s="122"/>
+      <c r="C307" s="125"/>
+      <c r="D307" s="125"/>
+      <c r="E307" s="125"/>
+      <c r="F307" s="115"/>
+      <c r="G307" s="115"/>
+      <c r="H307" s="116"/>
+      <c r="I307" s="115"/>
+      <c r="J307" s="115"/>
+      <c r="K307" s="115"/>
+      <c r="L307" s="115"/>
     </row>
     <row r="308" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A308" s="10" t="s">
@@ -14118,7 +14118,7 @@
       <c r="G308" s="102" t="s">
         <v>431</v>
       </c>
-      <c r="H308" s="124" t="s">
+      <c r="H308" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I308" s="27" t="s">
@@ -14152,7 +14152,7 @@
         <v>434</v>
       </c>
       <c r="G309" s="3"/>
-      <c r="H309" s="124" t="s">
+      <c r="H309" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I309" s="27" t="s">
@@ -14167,7 +14167,7 @@
       </c>
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A310" s="125">
+      <c r="A310" s="117">
         <v>113</v>
       </c>
       <c r="B310" s="12">
@@ -14186,10 +14186,10 @@
         <v>66</v>
       </c>
       <c r="G310" s="3"/>
-      <c r="H310" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I310" s="125" t="s">
+      <c r="H310" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I310" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J310" s="38" t="s">
@@ -14201,7 +14201,7 @@
       </c>
     </row>
     <row r="311" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A311" s="125">
+      <c r="A311" s="117">
         <v>113</v>
       </c>
       <c r="B311" s="93"/>
@@ -14220,22 +14220,22 @@
       <c r="G311" s="96" t="s">
         <v>238</v>
       </c>
-      <c r="H311" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I311" s="125" t="s">
+      <c r="H311" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I311" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J311" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K311" s="126"/>
-      <c r="L311" s="126">
+      <c r="K311" s="118"/>
+      <c r="L311" s="118">
         <v>0</v>
       </c>
     </row>
     <row r="312" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A312" s="125">
+      <c r="A312" s="117">
         <v>113</v>
       </c>
       <c r="B312" s="93"/>
@@ -14254,22 +14254,22 @@
       <c r="G312" s="96" t="s">
         <v>242</v>
       </c>
-      <c r="H312" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I312" s="125" t="s">
+      <c r="H312" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I312" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J312" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K312" s="126"/>
-      <c r="L312" s="126">
+      <c r="K312" s="118"/>
+      <c r="L312" s="118">
         <v>0</v>
       </c>
     </row>
     <row r="313" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A313" s="125">
+      <c r="A313" s="117">
         <v>113</v>
       </c>
       <c r="B313" s="99"/>
@@ -14288,22 +14288,22 @@
       <c r="G313" s="102" t="s">
         <v>245</v>
       </c>
-      <c r="H313" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I313" s="125" t="s">
+      <c r="H313" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I313" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J313" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K313" s="127"/>
-      <c r="L313" s="127">
+      <c r="K313" s="119"/>
+      <c r="L313" s="119">
         <v>0</v>
       </c>
     </row>
     <row r="314" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A314" s="125">
+      <c r="A314" s="117">
         <v>113</v>
       </c>
       <c r="B314" s="99"/>
@@ -14322,22 +14322,22 @@
       <c r="G314" s="102" t="s">
         <v>249</v>
       </c>
-      <c r="H314" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I314" s="125" t="s">
+      <c r="H314" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I314" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J314" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K314" s="127"/>
-      <c r="L314" s="127">
+      <c r="K314" s="119"/>
+      <c r="L314" s="119">
         <v>0</v>
       </c>
     </row>
     <row r="315" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A315" s="125">
+      <c r="A315" s="117">
         <v>113</v>
       </c>
       <c r="B315" s="99"/>
@@ -14356,17 +14356,17 @@
       <c r="G315" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="H315" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I315" s="125" t="s">
+      <c r="H315" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I315" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J315" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K315" s="127"/>
-      <c r="L315" s="127">
+      <c r="K315" s="119"/>
+      <c r="L315" s="119">
         <v>0</v>
       </c>
     </row>
@@ -14385,7 +14385,7 @@
       <c r="L316" s="39"/>
     </row>
     <row r="317" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A317" s="125">
+      <c r="A317" s="117">
         <v>113</v>
       </c>
       <c r="B317" s="99"/>
@@ -14404,22 +14404,22 @@
       <c r="G317" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="H317" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I317" s="125" t="s">
+      <c r="H317" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I317" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J317" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K317" s="127"/>
-      <c r="L317" s="127">
+      <c r="K317" s="119"/>
+      <c r="L317" s="119">
         <v>0</v>
       </c>
     </row>
     <row r="318" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A318" s="125">
+      <c r="A318" s="117">
         <v>113</v>
       </c>
       <c r="B318" s="93"/>
@@ -14438,22 +14438,22 @@
       <c r="G318" s="96" t="s">
         <v>249</v>
       </c>
-      <c r="H318" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I318" s="125" t="s">
+      <c r="H318" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I318" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J318" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K318" s="126"/>
-      <c r="L318" s="126">
+      <c r="K318" s="118"/>
+      <c r="L318" s="118">
         <v>0</v>
       </c>
     </row>
     <row r="319" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A319" s="125">
+      <c r="A319" s="117">
         <v>113</v>
       </c>
       <c r="B319" s="93"/>
@@ -14470,22 +14470,22 @@
         <v>441</v>
       </c>
       <c r="G319" s="96"/>
-      <c r="H319" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I319" s="125" t="s">
+      <c r="H319" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I319" s="117" t="s">
         <v>12</v>
       </c>
       <c r="J319" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K319" s="126"/>
-      <c r="L319" s="126">
+      <c r="K319" s="118"/>
+      <c r="L319" s="118">
         <v>0</v>
       </c>
     </row>
     <row r="320" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A320" s="125">
+      <c r="A320" s="117">
         <v>113</v>
       </c>
       <c r="B320" s="93"/>
@@ -14502,22 +14502,22 @@
         <v>268</v>
       </c>
       <c r="G320" s="96"/>
-      <c r="H320" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I320" s="125" t="s">
+      <c r="H320" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I320" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J320" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K320" s="126"/>
-      <c r="L320" s="126">
+      <c r="K320" s="118"/>
+      <c r="L320" s="118">
         <v>0</v>
       </c>
     </row>
     <row r="321" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A321" s="125">
+      <c r="A321" s="117">
         <v>113</v>
       </c>
       <c r="B321" s="99"/>
@@ -14536,22 +14536,22 @@
       <c r="G321" s="102" t="s">
         <v>249</v>
       </c>
-      <c r="H321" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I321" s="125" t="s">
+      <c r="H321" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I321" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J321" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K321" s="127"/>
-      <c r="L321" s="127">
+      <c r="K321" s="119"/>
+      <c r="L321" s="119">
         <v>0</v>
       </c>
     </row>
     <row r="322" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A322" s="125">
+      <c r="A322" s="117">
         <v>113</v>
       </c>
       <c r="B322" s="99"/>
@@ -14570,22 +14570,22 @@
       <c r="G322" s="102" t="s">
         <v>253</v>
       </c>
-      <c r="H322" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I322" s="125" t="s">
+      <c r="H322" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I322" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J322" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K322" s="127"/>
-      <c r="L322" s="127">
+      <c r="K322" s="119"/>
+      <c r="L322" s="119">
         <v>0</v>
       </c>
     </row>
     <row r="323" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A323" s="125">
+      <c r="A323" s="117">
         <v>113</v>
       </c>
       <c r="B323" s="12"/>
@@ -14604,10 +14604,10 @@
       <c r="G323" s="3" t="s">
         <v>279</v>
       </c>
-      <c r="H323" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="I323" s="125" t="s">
+      <c r="H323" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I323" s="117" t="s">
         <v>2</v>
       </c>
       <c r="J323" s="38" t="s">
@@ -14619,37 +14619,37 @@
       </c>
     </row>
     <row r="324" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A324" s="125"/>
+      <c r="A324" s="117"/>
       <c r="B324" s="12"/>
       <c r="C324" s="22"/>
       <c r="D324" s="23"/>
       <c r="E324" s="1"/>
       <c r="F324" s="24"/>
       <c r="G324" s="3"/>
-      <c r="H324" s="124"/>
-      <c r="I324" s="125"/>
+      <c r="H324" s="116"/>
+      <c r="I324" s="117"/>
       <c r="J324" s="38"/>
       <c r="K324" s="39"/>
       <c r="L324" s="39"/>
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A325" s="122"/>
-      <c r="B325" s="123" t="s">
+      <c r="A325" s="115"/>
+      <c r="B325" s="125" t="s">
         <v>444</v>
       </c>
-      <c r="C325" s="123"/>
-      <c r="D325" s="123"/>
-      <c r="E325" s="123"/>
-      <c r="F325" s="122"/>
-      <c r="G325" s="122"/>
-      <c r="H325" s="124"/>
-      <c r="I325" s="122"/>
-      <c r="J325" s="122"/>
-      <c r="K325" s="122"/>
-      <c r="L325" s="122"/>
+      <c r="C325" s="125"/>
+      <c r="D325" s="125"/>
+      <c r="E325" s="125"/>
+      <c r="F325" s="115"/>
+      <c r="G325" s="115"/>
+      <c r="H325" s="116"/>
+      <c r="I325" s="115"/>
+      <c r="J325" s="115"/>
+      <c r="K325" s="115"/>
+      <c r="L325" s="115"/>
     </row>
     <row r="326" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A326" s="125">
+      <c r="A326" s="117">
         <v>114</v>
       </c>
       <c r="B326" s="93"/>
@@ -14666,7 +14666,7 @@
         <v>282</v>
       </c>
       <c r="G326" s="96"/>
-      <c r="H326" s="124" t="s">
+      <c r="H326" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I326" s="93" t="s">
@@ -14675,13 +14675,13 @@
       <c r="J326" s="97" t="s">
         <v>12</v>
       </c>
-      <c r="K326" s="126"/>
+      <c r="K326" s="118"/>
       <c r="L326" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="327" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A327" s="125">
+      <c r="A327" s="117">
         <v>114</v>
       </c>
       <c r="B327" s="99"/>
@@ -14698,7 +14698,7 @@
         <v>285</v>
       </c>
       <c r="G327" s="102"/>
-      <c r="H327" s="124" t="s">
+      <c r="H327" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I327" s="99" t="s">
@@ -14707,13 +14707,13 @@
       <c r="J327" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K327" s="127"/>
+      <c r="K327" s="119"/>
       <c r="L327" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A328" s="125">
+      <c r="A328" s="117">
         <v>114</v>
       </c>
       <c r="B328" s="99"/>
@@ -14732,7 +14732,7 @@
       <c r="G328" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="H328" s="124" t="s">
+      <c r="H328" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I328" s="99" t="s">
@@ -14741,13 +14741,13 @@
       <c r="J328" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K328" s="127"/>
+      <c r="K328" s="119"/>
       <c r="L328" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="329" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A329" s="125">
+      <c r="A329" s="117">
         <v>114</v>
       </c>
       <c r="B329" s="99"/>
@@ -14764,7 +14764,7 @@
         <v>289</v>
       </c>
       <c r="G329" s="102"/>
-      <c r="H329" s="124" t="s">
+      <c r="H329" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I329" s="99" t="s">
@@ -14773,13 +14773,13 @@
       <c r="J329" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K329" s="127"/>
+      <c r="K329" s="119"/>
       <c r="L329" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="330" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A330" s="125">
+      <c r="A330" s="117">
         <v>114</v>
       </c>
       <c r="B330" s="99"/>
@@ -14798,7 +14798,7 @@
       <c r="G330" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="H330" s="124" t="s">
+      <c r="H330" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I330" s="99" t="s">
@@ -14807,13 +14807,13 @@
       <c r="J330" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K330" s="127"/>
+      <c r="K330" s="119"/>
       <c r="L330" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="331" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A331" s="125">
+      <c r="A331" s="117">
         <v>114</v>
       </c>
       <c r="B331" s="99"/>
@@ -14830,7 +14830,7 @@
         <v>293</v>
       </c>
       <c r="G331" s="102"/>
-      <c r="H331" s="124" t="s">
+      <c r="H331" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I331" s="99" t="s">
@@ -14839,13 +14839,13 @@
       <c r="J331" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K331" s="127"/>
+      <c r="K331" s="119"/>
       <c r="L331" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="332" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A332" s="125">
+      <c r="A332" s="117">
         <v>114</v>
       </c>
       <c r="B332" s="99"/>
@@ -14864,7 +14864,7 @@
       <c r="G332" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="H332" s="124" t="s">
+      <c r="H332" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I332" s="99" t="s">
@@ -14873,7 +14873,7 @@
       <c r="J332" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K332" s="127"/>
+      <c r="K332" s="119"/>
       <c r="L332" s="39">
         <v>0</v>
       </c>
@@ -14893,7 +14893,7 @@
       <c r="L333" s="39"/>
     </row>
     <row r="334" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A334" s="125">
+      <c r="A334" s="117">
         <v>114</v>
       </c>
       <c r="B334" s="99"/>
@@ -14912,7 +14912,7 @@
       <c r="G334" s="102" t="s">
         <v>260</v>
       </c>
-      <c r="H334" s="124" t="s">
+      <c r="H334" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I334" s="99" t="s">
@@ -14921,13 +14921,13 @@
       <c r="J334" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="K334" s="127"/>
+      <c r="K334" s="119"/>
       <c r="L334" s="39">
         <v>0</v>
       </c>
     </row>
     <row r="335" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A335" s="125">
+      <c r="A335" s="117">
         <v>114</v>
       </c>
       <c r="B335" s="99"/>
@@ -14946,7 +14946,7 @@
       <c r="G335" s="102" t="s">
         <v>299</v>
       </c>
-      <c r="H335" s="128" t="s">
+      <c r="H335" s="120" t="s">
         <v>12</v>
       </c>
       <c r="I335" s="99" t="s">
@@ -14961,24 +14961,24 @@
       </c>
     </row>
     <row r="336" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A336" s="125">
+      <c r="A336" s="117">
         <v>114</v>
       </c>
       <c r="B336" s="12"/>
       <c r="C336" s="39"/>
-      <c r="D336" s="129" t="s">
+      <c r="D336" s="121" t="s">
         <v>307</v>
       </c>
       <c r="E336" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F336" s="130" t="s">
+      <c r="F336" s="122" t="s">
         <v>308</v>
       </c>
       <c r="G336" s="40" t="s">
         <v>309</v>
       </c>
-      <c r="H336" s="124" t="s">
+      <c r="H336" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I336" s="27" t="s">
@@ -14991,7 +14991,7 @@
       </c>
     </row>
     <row r="337" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A337" s="125">
+      <c r="A337" s="117">
         <v>114</v>
       </c>
       <c r="B337" s="12"/>
@@ -15006,7 +15006,7 @@
       <c r="G337" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="H337" s="124" t="s">
+      <c r="H337" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I337" s="27" t="s">
@@ -15021,26 +15021,26 @@
       </c>
     </row>
     <row r="338" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A338" s="125">
+      <c r="A338" s="117">
         <v>114</v>
       </c>
       <c r="B338" s="12"/>
       <c r="C338" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="D338" s="129" t="s">
+      <c r="D338" s="121" t="s">
         <v>314</v>
       </c>
       <c r="E338" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F338" s="130" t="s">
+      <c r="F338" s="122" t="s">
         <v>315</v>
       </c>
       <c r="G338" s="40" t="s">
         <v>316</v>
       </c>
-      <c r="H338" s="124" t="s">
+      <c r="H338" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I338" s="27" t="s">
@@ -15053,24 +15053,24 @@
       </c>
     </row>
     <row r="339" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A339" s="125">
+      <c r="A339" s="117">
         <v>114</v>
       </c>
       <c r="B339" s="12"/>
       <c r="C339" s="22"/>
-      <c r="D339" s="129" t="s">
+      <c r="D339" s="121" t="s">
         <v>317</v>
       </c>
       <c r="E339" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F339" s="130" t="s">
+      <c r="F339" s="122" t="s">
         <v>318</v>
       </c>
       <c r="G339" s="40" t="s">
         <v>319</v>
       </c>
-      <c r="H339" s="124" t="s">
+      <c r="H339" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I339" s="27" t="s">
@@ -15083,7 +15083,7 @@
       </c>
     </row>
     <row r="340" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A340" s="125">
+      <c r="A340" s="117">
         <v>114</v>
       </c>
       <c r="B340" s="12"/>
@@ -15098,7 +15098,7 @@
       <c r="G340" s="3" t="s">
         <v>320</v>
       </c>
-      <c r="H340" s="124" t="s">
+      <c r="H340" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I340" s="27" t="s">
@@ -15113,26 +15113,26 @@
       </c>
     </row>
     <row r="341" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A341" s="125">
+      <c r="A341" s="117">
         <v>114</v>
       </c>
       <c r="B341" s="12"/>
       <c r="C341" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="D341" s="129" t="s">
+      <c r="D341" s="121" t="s">
         <v>322</v>
       </c>
       <c r="E341" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F341" s="130" t="s">
+      <c r="F341" s="122" t="s">
         <v>323</v>
       </c>
       <c r="G341" s="40" t="s">
         <v>324</v>
       </c>
-      <c r="H341" s="124" t="s">
+      <c r="H341" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I341" s="27" t="s">
@@ -15145,24 +15145,24 @@
       </c>
     </row>
     <row r="342" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A342" s="125">
+      <c r="A342" s="117">
         <v>114</v>
       </c>
       <c r="B342" s="12"/>
-      <c r="C342" s="131"/>
-      <c r="D342" s="129" t="s">
+      <c r="C342" s="123"/>
+      <c r="D342" s="121" t="s">
         <v>325</v>
       </c>
       <c r="E342" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F342" s="130" t="s">
+      <c r="F342" s="122" t="s">
         <v>326</v>
       </c>
       <c r="G342" s="40" t="s">
         <v>327</v>
       </c>
-      <c r="H342" s="124" t="s">
+      <c r="H342" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I342" s="27" t="s">
@@ -15177,7 +15177,7 @@
       </c>
     </row>
     <row r="343" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A343" s="125">
+      <c r="A343" s="117">
         <v>114</v>
       </c>
       <c r="B343" s="12"/>
@@ -15192,7 +15192,7 @@
       <c r="G343" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="H343" s="124" t="s">
+      <c r="H343" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I343" s="27" t="s">
@@ -15207,7 +15207,7 @@
       </c>
     </row>
     <row r="344" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A344" s="125">
+      <c r="A344" s="117">
         <v>114</v>
       </c>
       <c r="B344" s="12">
@@ -15216,19 +15216,19 @@
       <c r="C344" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="D344" s="129" t="s">
+      <c r="D344" s="121" t="s">
         <v>107</v>
       </c>
       <c r="E344" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F344" s="130" t="s">
+      <c r="F344" s="122" t="s">
         <v>109</v>
       </c>
       <c r="G344" s="40">
         <v>0</v>
       </c>
-      <c r="H344" s="124" t="s">
+      <c r="H344" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I344" s="27" t="s">
@@ -15243,7 +15243,7 @@
       </c>
     </row>
     <row r="345" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A345" s="125">
+      <c r="A345" s="117">
         <v>114</v>
       </c>
       <c r="B345" s="12">
@@ -15252,19 +15252,19 @@
       <c r="C345" s="22" t="s">
         <v>332</v>
       </c>
-      <c r="D345" s="129" t="s">
+      <c r="D345" s="121" t="s">
         <v>333</v>
       </c>
       <c r="E345" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F345" s="130" t="s">
+      <c r="F345" s="122" t="s">
         <v>113</v>
       </c>
       <c r="G345" s="40">
         <v>0</v>
       </c>
-      <c r="H345" s="124" t="s">
+      <c r="H345" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I345" s="27" t="s">
@@ -15279,7 +15279,7 @@
       </c>
     </row>
     <row r="346" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A346" s="125">
+      <c r="A346" s="117">
         <v>114</v>
       </c>
       <c r="B346" s="12">
@@ -15288,19 +15288,19 @@
       <c r="C346" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="D346" s="129" t="s">
+      <c r="D346" s="121" t="s">
         <v>335</v>
       </c>
       <c r="E346" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F346" s="130" t="s">
+      <c r="F346" s="122" t="s">
         <v>117</v>
       </c>
       <c r="G346" s="40">
         <v>0</v>
       </c>
-      <c r="H346" s="124" t="s">
+      <c r="H346" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I346" s="27" t="s">
@@ -15315,7 +15315,7 @@
       </c>
     </row>
     <row r="347" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A347" s="125">
+      <c r="A347" s="117">
         <v>114</v>
       </c>
       <c r="B347" s="12">
@@ -15324,19 +15324,19 @@
       <c r="C347" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="D347" s="129" t="s">
+      <c r="D347" s="121" t="s">
         <v>337</v>
       </c>
       <c r="E347" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F347" s="130" t="s">
+      <c r="F347" s="122" t="s">
         <v>338</v>
       </c>
       <c r="G347" s="40">
         <v>0</v>
       </c>
-      <c r="H347" s="124" t="s">
+      <c r="H347" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I347" s="27" t="s">
@@ -15351,7 +15351,7 @@
       </c>
     </row>
     <row r="348" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A348" s="125">
+      <c r="A348" s="117">
         <v>114</v>
       </c>
       <c r="B348" s="12">
@@ -15360,17 +15360,17 @@
       <c r="C348" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="D348" s="129" t="s">
+      <c r="D348" s="121" t="s">
         <v>337</v>
       </c>
       <c r="E348" s="1" t="s">
         <v>264</v>
       </c>
-      <c r="F348" s="130" t="s">
+      <c r="F348" s="122" t="s">
         <v>338</v>
       </c>
       <c r="G348" s="40"/>
-      <c r="H348" s="124" t="s">
+      <c r="H348" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I348" s="27" t="s">
@@ -15385,24 +15385,24 @@
       </c>
     </row>
     <row r="349" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A349" s="125">
+      <c r="A349" s="117">
         <v>114</v>
       </c>
       <c r="B349" s="12"/>
-      <c r="C349" s="131"/>
-      <c r="D349" s="129" t="s">
+      <c r="C349" s="123"/>
+      <c r="D349" s="121" t="s">
         <v>341</v>
       </c>
       <c r="E349" s="1" t="s">
         <v>297</v>
       </c>
-      <c r="F349" s="130" t="s">
+      <c r="F349" s="122" t="s">
         <v>342</v>
       </c>
       <c r="G349" s="40" t="s">
         <v>343</v>
       </c>
-      <c r="H349" s="124" t="s">
+      <c r="H349" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I349" s="27" t="s">
@@ -15417,24 +15417,24 @@
       </c>
     </row>
     <row r="350" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A350" s="125">
+      <c r="A350" s="117">
         <v>114</v>
       </c>
       <c r="B350" s="12"/>
-      <c r="C350" s="131" t="s">
+      <c r="C350" s="123" t="s">
         <v>340</v>
       </c>
-      <c r="D350" s="129" t="s">
+      <c r="D350" s="121" t="s">
         <v>344</v>
       </c>
       <c r="E350" s="1" t="s">
         <v>311</v>
       </c>
-      <c r="F350" s="130"/>
+      <c r="F350" s="122"/>
       <c r="G350" s="40" t="s">
         <v>345</v>
       </c>
-      <c r="H350" s="124" t="s">
+      <c r="H350" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I350" s="27" t="s">
@@ -15449,7 +15449,7 @@
       </c>
     </row>
     <row r="351" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A351" s="125">
+      <c r="A351" s="117">
         <v>114</v>
       </c>
       <c r="B351" s="35"/>
@@ -15466,7 +15466,7 @@
         <v>101</v>
       </c>
       <c r="G351" s="41"/>
-      <c r="H351" s="124" t="s">
+      <c r="H351" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I351" s="27" t="s">
@@ -15483,7 +15483,7 @@
       </c>
     </row>
     <row r="352" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A352" s="125">
+      <c r="A352" s="117">
         <v>114</v>
       </c>
       <c r="B352" s="35"/>
@@ -15500,7 +15500,7 @@
         <v>352</v>
       </c>
       <c r="G352" s="41"/>
-      <c r="H352" s="124" t="s">
+      <c r="H352" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I352" s="27" t="s">
@@ -15517,7 +15517,7 @@
       </c>
     </row>
     <row r="353" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A353" s="125">
+      <c r="A353" s="117">
         <v>114</v>
       </c>
       <c r="B353" s="35"/>
@@ -15534,7 +15534,7 @@
         <v>356</v>
       </c>
       <c r="G353" s="41"/>
-      <c r="H353" s="124" t="s">
+      <c r="H353" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I353" s="27" t="s">
@@ -15551,7 +15551,7 @@
       </c>
     </row>
     <row r="354" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A354" s="125">
+      <c r="A354" s="117">
         <v>114</v>
       </c>
       <c r="B354" s="35"/>
@@ -15568,7 +15568,7 @@
         <v>125</v>
       </c>
       <c r="G354" s="41"/>
-      <c r="H354" s="124" t="s">
+      <c r="H354" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I354" s="27" t="s">
@@ -15585,7 +15585,7 @@
       </c>
     </row>
     <row r="355" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A355" s="125">
+      <c r="A355" s="117">
         <v>114</v>
       </c>
       <c r="B355" s="35"/>
@@ -15602,7 +15602,7 @@
         <v>361</v>
       </c>
       <c r="G355" s="41"/>
-      <c r="H355" s="124" t="s">
+      <c r="H355" s="116" t="s">
         <v>12</v>
       </c>
       <c r="I355" s="27" t="s">
@@ -15633,20 +15633,20 @@
       <c r="L356" s="39"/>
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A357" s="122"/>
-      <c r="B357" s="123" t="s">
+      <c r="A357" s="115"/>
+      <c r="B357" s="125" t="s">
         <v>446</v>
       </c>
-      <c r="C357" s="123"/>
-      <c r="D357" s="123"/>
-      <c r="E357" s="123"/>
-      <c r="F357" s="122"/>
-      <c r="G357" s="122"/>
-      <c r="H357" s="124"/>
-      <c r="I357" s="122"/>
-      <c r="J357" s="122"/>
-      <c r="K357" s="122"/>
-      <c r="L357" s="122"/>
+      <c r="C357" s="125"/>
+      <c r="D357" s="125"/>
+      <c r="E357" s="125"/>
+      <c r="F357" s="115"/>
+      <c r="G357" s="115"/>
+      <c r="H357" s="116"/>
+      <c r="I357" s="115"/>
+      <c r="J357" s="115"/>
+      <c r="K357" s="115"/>
+      <c r="L357" s="115"/>
     </row>
     <row r="358" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A358" s="10" t="s">
@@ -15670,7 +15670,7 @@
       <c r="G358" s="3" t="s">
         <v>448</v>
       </c>
-      <c r="H358" s="124" t="s">
+      <c r="H358" s="116" t="s">
         <v>2</v>
       </c>
       <c r="I358" s="40" t="s">
@@ -15963,7 +15963,7 @@
       <c r="B367" s="12">
         <v>6</v>
       </c>
-      <c r="C367" s="132" t="s">
+      <c r="C367" s="124" t="s">
         <v>460</v>
       </c>
       <c r="D367" s="20" t="s">
@@ -16014,7 +16014,7 @@
       </c>
       <c r="H368" s="1"/>
       <c r="I368" s="27" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="J368" s="47" t="s">
         <v>12</v>
@@ -16094,21 +16094,21 @@
     </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C124:J124"/>
+    <mergeCell ref="B167:D167"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="B217:D217"/>
+    <mergeCell ref="B251:D251"/>
+    <mergeCell ref="B264:D264"/>
     <mergeCell ref="B307:E307"/>
     <mergeCell ref="B325:E325"/>
     <mergeCell ref="B357:E357"/>
     <mergeCell ref="B288:D288"/>
     <mergeCell ref="B298:D298"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="B217:D217"/>
-    <mergeCell ref="B251:D251"/>
-    <mergeCell ref="B264:D264"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C124:J124"/>
-    <mergeCell ref="B167:D167"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="370" priority="405" operator="equal">
@@ -16813,158 +16813,158 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H359">
-    <cfRule type="cellIs" dxfId="47" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="48" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H359">
-    <cfRule type="cellIs" dxfId="46" priority="46" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="207" priority="46" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="206" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H360">
-    <cfRule type="cellIs" dxfId="44" priority="44" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="44" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H360">
-    <cfRule type="cellIs" dxfId="43" priority="42" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="204" priority="42" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="203" priority="43" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H361">
-    <cfRule type="cellIs" dxfId="41" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="40" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H361">
-    <cfRule type="cellIs" dxfId="40" priority="38" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="201" priority="38" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="200" priority="39" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H362">
-    <cfRule type="cellIs" dxfId="38" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="36" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H362">
-    <cfRule type="cellIs" dxfId="37" priority="34" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="35" operator="equal">
+    <cfRule type="cellIs" dxfId="198" priority="34" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="197" priority="35" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H363">
-    <cfRule type="cellIs" dxfId="35" priority="32" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="32" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H363">
-    <cfRule type="cellIs" dxfId="34" priority="30" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="195" priority="30" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="194" priority="31" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H364">
-    <cfRule type="cellIs" dxfId="32" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="28" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H364">
-    <cfRule type="cellIs" dxfId="31" priority="26" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="30" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="192" priority="26" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="191" priority="27" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H366">
-    <cfRule type="cellIs" dxfId="29" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H366">
-    <cfRule type="cellIs" dxfId="28" priority="22" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="189" priority="22" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="188" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H367">
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="20" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H367">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="186" priority="18" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="185" priority="19" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H368">
-    <cfRule type="cellIs" dxfId="23" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="16" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H368">
-    <cfRule type="cellIs" dxfId="22" priority="14" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="183" priority="14" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="182" priority="15" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H369">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="12" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H369">
-    <cfRule type="cellIs" dxfId="19" priority="10" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="180" priority="10" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="179" priority="11" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H370">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="8" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H370">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="177" priority="6" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="176" priority="7" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H365">
-    <cfRule type="cellIs" dxfId="14" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="4" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H365">
-    <cfRule type="cellIs" dxfId="13" priority="2" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
+      <formula>#REF!</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="173" priority="3" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Resolve Login issue for Edge and IE
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-3780" windowWidth="29040" windowHeight="15840" activeTab="1"/>
+    <workbookView xWindow="-28920" yWindow="-3330" windowWidth="29040" windowHeight="15840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2334" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2346" uniqueCount="467">
   <si>
     <t>Action</t>
   </si>
@@ -1423,10 +1423,10 @@
     <t>Verify Revision Adj amount</t>
   </si>
   <si>
-    <t>Revision,$revision,Rev Adj. Amount,$0.00</t>
-  </si>
-  <si>
     <t>Common Part 3 Add Revision</t>
+  </si>
+  <si>
+    <t>Revision,$revision,Rev Adj. Amount,0.00</t>
   </si>
 </sst>
 </file>
@@ -2012,13 +2012,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2030,10 +2030,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -5290,7 +5290,7 @@
         <v>115</v>
       </c>
       <c r="C16" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="D16" s="2" t="s">
         <v>2</v>
@@ -5307,10 +5307,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L370"/>
+  <dimension ref="A1:L371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F345" workbookViewId="0">
-      <selection activeCell="I368" sqref="I368"/>
+    <sheetView tabSelected="1" topLeftCell="F342" workbookViewId="0">
+      <selection activeCell="I370" sqref="I370"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5367,16 +5367,16 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
-      <c r="C2" s="131" t="s">
+      <c r="C2" s="125" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="131"/>
-      <c r="E2" s="131"/>
-      <c r="F2" s="131"/>
-      <c r="G2" s="131"/>
-      <c r="H2" s="131"/>
-      <c r="I2" s="131"/>
-      <c r="J2" s="131"/>
+      <c r="D2" s="125"/>
+      <c r="E2" s="125"/>
+      <c r="F2" s="125"/>
+      <c r="G2" s="125"/>
+      <c r="H2" s="125"/>
+      <c r="I2" s="125"/>
+      <c r="J2" s="125"/>
       <c r="K2" s="32"/>
       <c r="L2" s="33"/>
     </row>
@@ -6486,16 +6486,16 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39" s="31"/>
       <c r="B39" s="32"/>
-      <c r="C39" s="131" t="s">
+      <c r="C39" s="125" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="131"/>
-      <c r="E39" s="131"/>
-      <c r="F39" s="131"/>
-      <c r="G39" s="131"/>
-      <c r="H39" s="131"/>
-      <c r="I39" s="131"/>
-      <c r="J39" s="131"/>
+      <c r="D39" s="125"/>
+      <c r="E39" s="125"/>
+      <c r="F39" s="125"/>
+      <c r="G39" s="125"/>
+      <c r="H39" s="125"/>
+      <c r="I39" s="125"/>
+      <c r="J39" s="125"/>
       <c r="K39" s="32"/>
       <c r="L39" s="33"/>
     </row>
@@ -7671,16 +7671,16 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79" s="31"/>
       <c r="B79" s="32"/>
-      <c r="C79" s="131" t="s">
+      <c r="C79" s="125" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="131"/>
-      <c r="E79" s="131"/>
-      <c r="F79" s="131"/>
-      <c r="G79" s="131"/>
-      <c r="H79" s="131"/>
-      <c r="I79" s="131"/>
-      <c r="J79" s="131"/>
+      <c r="D79" s="125"/>
+      <c r="E79" s="125"/>
+      <c r="F79" s="125"/>
+      <c r="G79" s="125"/>
+      <c r="H79" s="125"/>
+      <c r="I79" s="125"/>
+      <c r="J79" s="125"/>
       <c r="K79" s="32"/>
       <c r="L79" s="33"/>
     </row>
@@ -8955,16 +8955,16 @@
     <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124" s="31"/>
       <c r="B124" s="32"/>
-      <c r="C124" s="131" t="s">
+      <c r="C124" s="125" t="s">
         <v>198</v>
       </c>
-      <c r="D124" s="131"/>
-      <c r="E124" s="131"/>
-      <c r="F124" s="131"/>
-      <c r="G124" s="131"/>
-      <c r="H124" s="131"/>
-      <c r="I124" s="131"/>
-      <c r="J124" s="131"/>
+      <c r="D124" s="125"/>
+      <c r="E124" s="125"/>
+      <c r="F124" s="125"/>
+      <c r="G124" s="125"/>
+      <c r="H124" s="125"/>
+      <c r="I124" s="125"/>
+      <c r="J124" s="125"/>
       <c r="K124" s="32"/>
       <c r="L124" s="33"/>
     </row>
@@ -10221,11 +10221,11 @@
       </c>
     </row>
     <row r="167" spans="1:12" s="77" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B167" s="132" t="s">
+      <c r="B167" s="126" t="s">
         <v>206</v>
       </c>
-      <c r="C167" s="132"/>
-      <c r="D167" s="132"/>
+      <c r="C167" s="126"/>
+      <c r="D167" s="126"/>
       <c r="H167" s="78"/>
     </row>
     <row r="168" spans="1:12" x14ac:dyDescent="0.25">
@@ -10704,11 +10704,11 @@
       <c r="J183" s="18"/>
     </row>
     <row r="184" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B184" s="126" t="s">
+      <c r="B184" s="127" t="s">
         <v>211</v>
       </c>
-      <c r="C184" s="126"/>
-      <c r="D184" s="126"/>
+      <c r="C184" s="127"/>
+      <c r="D184" s="127"/>
       <c r="H184" s="86"/>
     </row>
     <row r="185" spans="1:12" x14ac:dyDescent="0.25">
@@ -13547,11 +13547,11 @@
       </c>
     </row>
     <row r="288" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B288" s="126" t="s">
+      <c r="B288" s="127" t="s">
         <v>415</v>
       </c>
-      <c r="C288" s="126"/>
-      <c r="D288" s="126"/>
+      <c r="C288" s="127"/>
+      <c r="D288" s="127"/>
       <c r="H288" s="86"/>
     </row>
     <row r="289" spans="1:12" x14ac:dyDescent="0.25">
@@ -13830,11 +13830,11 @@
       </c>
     </row>
     <row r="298" spans="1:12" s="85" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B298" s="127" t="s">
+      <c r="B298" s="132" t="s">
         <v>414</v>
       </c>
-      <c r="C298" s="127"/>
-      <c r="D298" s="127"/>
+      <c r="C298" s="132"/>
+      <c r="D298" s="132"/>
       <c r="H298" s="86"/>
     </row>
     <row r="299" spans="1:12" x14ac:dyDescent="0.25">
@@ -14082,12 +14082,12 @@
     </row>
     <row r="307" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A307" s="115"/>
-      <c r="B307" s="125" t="s">
+      <c r="B307" s="131" t="s">
         <v>427</v>
       </c>
-      <c r="C307" s="125"/>
-      <c r="D307" s="125"/>
-      <c r="E307" s="125"/>
+      <c r="C307" s="131"/>
+      <c r="D307" s="131"/>
+      <c r="E307" s="131"/>
       <c r="F307" s="115"/>
       <c r="G307" s="115"/>
       <c r="H307" s="116"/>
@@ -14634,12 +14634,12 @@
     </row>
     <row r="325" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A325" s="115"/>
-      <c r="B325" s="125" t="s">
+      <c r="B325" s="131" t="s">
         <v>444</v>
       </c>
-      <c r="C325" s="125"/>
-      <c r="D325" s="125"/>
-      <c r="E325" s="125"/>
+      <c r="C325" s="131"/>
+      <c r="D325" s="131"/>
+      <c r="E325" s="131"/>
       <c r="F325" s="115"/>
       <c r="G325" s="115"/>
       <c r="H325" s="116"/>
@@ -15634,12 +15634,12 @@
     </row>
     <row r="357" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A357" s="115"/>
-      <c r="B357" s="125" t="s">
+      <c r="B357" s="131" t="s">
         <v>446</v>
       </c>
-      <c r="C357" s="125"/>
-      <c r="D357" s="125"/>
-      <c r="E357" s="125"/>
+      <c r="C357" s="131"/>
+      <c r="D357" s="131"/>
+      <c r="E357" s="131"/>
       <c r="F357" s="115"/>
       <c r="G357" s="115"/>
       <c r="H357" s="116"/>
@@ -15706,7 +15706,9 @@
       <c r="G359" s="3" t="s">
         <v>450</v>
       </c>
-      <c r="H359" s="1"/>
+      <c r="H359" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I359" s="27" t="s">
         <v>12</v>
       </c>
@@ -15740,7 +15742,9 @@
       <c r="G360" s="3" t="s">
         <v>451</v>
       </c>
-      <c r="H360" s="1"/>
+      <c r="H360" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I360" s="17" t="s">
         <v>2</v>
       </c>
@@ -15774,7 +15778,9 @@
       <c r="G361" s="3" t="s">
         <v>452</v>
       </c>
-      <c r="H361" s="1"/>
+      <c r="H361" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I361" s="17" t="s">
         <v>2</v>
       </c>
@@ -15808,7 +15814,9 @@
       <c r="G362" s="3" t="s">
         <v>453</v>
       </c>
-      <c r="H362" s="1"/>
+      <c r="H362" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I362" s="17" t="s">
         <v>2</v>
       </c>
@@ -15842,7 +15850,9 @@
       <c r="G363" s="3" t="s">
         <v>454</v>
       </c>
-      <c r="H363" s="1"/>
+      <c r="H363" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I363" s="17" t="s">
         <v>2</v>
       </c>
@@ -15876,7 +15886,9 @@
       <c r="G364" s="3" t="s">
         <v>455</v>
       </c>
-      <c r="H364" s="1"/>
+      <c r="H364" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I364" s="17" t="s">
         <v>2</v>
       </c>
@@ -15910,7 +15922,9 @@
       <c r="G365" s="3" t="s">
         <v>458</v>
       </c>
-      <c r="H365" s="1"/>
+      <c r="H365" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I365" s="17" t="s">
         <v>2</v>
       </c>
@@ -15944,7 +15958,9 @@
       <c r="G366" s="3" t="s">
         <v>459</v>
       </c>
-      <c r="H366" s="1"/>
+      <c r="H366" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I366" s="17" t="s">
         <v>2</v>
       </c>
@@ -15978,8 +15994,10 @@
       <c r="G367" s="3" t="s">
         <v>461</v>
       </c>
-      <c r="H367" s="1"/>
-      <c r="I367" s="17" t="s">
+      <c r="H367" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I367" s="27" t="s">
         <v>2</v>
       </c>
       <c r="J367" s="47" t="s">
@@ -16012,7 +16030,9 @@
       <c r="G368" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="H368" s="1"/>
+      <c r="H368" s="116" t="s">
+        <v>12</v>
+      </c>
       <c r="I368" s="27" t="s">
         <v>2</v>
       </c>
@@ -16046,9 +16066,11 @@
       <c r="G369" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="H369" s="1"/>
-      <c r="I369" s="17" t="s">
-        <v>2</v>
+      <c r="H369" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I369" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="J369" s="47" t="s">
         <v>12</v>
@@ -16078,11 +16100,13 @@
         <v>39</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>465</v>
-      </c>
-      <c r="H370" s="1"/>
-      <c r="I370" s="17" t="s">
-        <v>2</v>
+        <v>466</v>
+      </c>
+      <c r="H370" s="116" t="s">
+        <v>12</v>
+      </c>
+      <c r="I370" s="27" t="s">
+        <v>12</v>
       </c>
       <c r="J370" s="47" t="s">
         <v>12</v>
@@ -16092,23 +16116,26 @@
         <v>0</v>
       </c>
     </row>
+    <row r="371" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H371" s="116"/>
+    </row>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="B307:E307"/>
+    <mergeCell ref="B325:E325"/>
+    <mergeCell ref="B357:E357"/>
+    <mergeCell ref="B288:D288"/>
+    <mergeCell ref="B298:D298"/>
+    <mergeCell ref="B184:D184"/>
+    <mergeCell ref="B198:D198"/>
+    <mergeCell ref="B217:D217"/>
+    <mergeCell ref="B251:D251"/>
+    <mergeCell ref="B264:D264"/>
     <mergeCell ref="C2:J2"/>
     <mergeCell ref="C39:J39"/>
     <mergeCell ref="C79:J79"/>
     <mergeCell ref="C124:J124"/>
     <mergeCell ref="B167:D167"/>
-    <mergeCell ref="B184:D184"/>
-    <mergeCell ref="B198:D198"/>
-    <mergeCell ref="B217:D217"/>
-    <mergeCell ref="B251:D251"/>
-    <mergeCell ref="B264:D264"/>
-    <mergeCell ref="B307:E307"/>
-    <mergeCell ref="B325:E325"/>
-    <mergeCell ref="B357:E357"/>
-    <mergeCell ref="B288:D288"/>
-    <mergeCell ref="B298:D298"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="370" priority="405" operator="equal">
@@ -16812,167 +16839,8 @@
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H359">
-    <cfRule type="cellIs" dxfId="208" priority="48" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H359">
-    <cfRule type="cellIs" dxfId="207" priority="46" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="47" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H360">
-    <cfRule type="cellIs" dxfId="205" priority="44" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H360">
-    <cfRule type="cellIs" dxfId="204" priority="42" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="43" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H361">
-    <cfRule type="cellIs" dxfId="202" priority="40" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H361">
-    <cfRule type="cellIs" dxfId="201" priority="38" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="39" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H362">
-    <cfRule type="cellIs" dxfId="199" priority="36" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H362">
-    <cfRule type="cellIs" dxfId="198" priority="34" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="35" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H363">
-    <cfRule type="cellIs" dxfId="196" priority="32" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H363">
-    <cfRule type="cellIs" dxfId="195" priority="30" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="31" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H364">
-    <cfRule type="cellIs" dxfId="193" priority="28" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H364">
-    <cfRule type="cellIs" dxfId="192" priority="26" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="27" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H366">
-    <cfRule type="cellIs" dxfId="190" priority="24" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H366">
-    <cfRule type="cellIs" dxfId="189" priority="22" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="23" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H367">
-    <cfRule type="cellIs" dxfId="187" priority="20" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H367">
-    <cfRule type="cellIs" dxfId="186" priority="18" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="19" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H368">
-    <cfRule type="cellIs" dxfId="184" priority="16" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H368">
-    <cfRule type="cellIs" dxfId="183" priority="14" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="15" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H369">
-    <cfRule type="cellIs" dxfId="181" priority="12" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H369">
-    <cfRule type="cellIs" dxfId="180" priority="10" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="11" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H370">
-    <cfRule type="cellIs" dxfId="178" priority="8" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H370">
-    <cfRule type="cellIs" dxfId="177" priority="6" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="7" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H365">
-    <cfRule type="cellIs" dxfId="175" priority="4" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="H365">
-    <cfRule type="cellIs" dxfId="174" priority="2" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="3" operator="equal">
-      <formula>#REF!</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
+  <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H149:H152 H185:H193 H60:H65 H57 H105:H108 H168:H183 H214:H215 H200:H201 H249:H250 H232 H235 H229 H257:H263 H275:H287 H265:H266 H289:H290 H299:H300 H252 H26">
-      <formula1>#REF!</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H359:H370">
       <formula1>#REF!</formula1>
     </dataValidation>
   </dataValidations>
@@ -19074,162 +18942,6 @@
           </x14:cfRule>
           <xm:sqref>H23:H25</xm:sqref>
         </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="45" operator="equal" id="{00C4F72D-025F-43D3-BEFC-7008F5900837}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H359</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="41" operator="equal" id="{7492812D-1B9A-40A6-8B3D-1F60652E47D7}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H360</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="37" operator="equal" id="{72666761-D695-4CEC-B3D5-6E5051729CC9}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H361</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="33" operator="equal" id="{6C51A7B2-1AC2-4035-818C-C48B99D25972}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H362</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="29" operator="equal" id="{82D9EC7F-9CC2-432A-8D83-6E9D4332FA3A}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H363</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="25" operator="equal" id="{8C51DFEC-3313-4BAE-B217-89BFD3A5274E}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H364</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="21" operator="equal" id="{BE650146-F2DA-4952-87C2-7A8CC98687BC}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H366</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="17" operator="equal" id="{6CC4CF67-54EF-4ADD-97D6-CA12FDEE3E3B}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H367</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="13" operator="equal" id="{D4D8B286-3AE0-4236-A558-A82C6834D7CD}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H368</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="9" operator="equal" id="{CCF98C23-7DA1-4A78-A374-30C9C8061AFE}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H369</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="5" operator="equal" id="{328F12C8-781F-4A1A-8E64-6CF8D287525F}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H370</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="1" operator="equal" id="{BB08CC85-3E8F-4588-B167-225385799277}">
-            <xm:f>'C:\Users\naveeng\Documents\Builds\AMTDirectAutomationSuite11\AMTDirectAutomationSuite\Framework\Modules\[PortFolioInsight.xlsx]Controller'!#REF!</xm:f>
-            <x14:dxf>
-              <fill>
-                <patternFill>
-                  <bgColor theme="5" tint="0.39994506668294322"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>H365</xm:sqref>
-        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>

</xml_diff>

<commit_message>
FRAT Updated : New Payment Check Method: InProgress
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAB354F4-E5EA-214E-8B5B-23E42ED0246C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84399283-AF0B-804C-9E88-237921DA1EDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3291" uniqueCount="565">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="564">
   <si>
     <t>Action</t>
   </si>
@@ -1527,18 +1527,6 @@
     <t>FASB.FISchedule.TemporaryLeaseSelection</t>
   </si>
   <si>
-    <t>- Adjusted NPV Interest Rate should be present</t>
-  </si>
-  <si>
-    <t>- Amortization Expense Per Day should be present</t>
-  </si>
-  <si>
-    <t>- Rent Expense Per Day should be present</t>
-  </si>
-  <si>
-    <t>- Display dropdown should populate FASB - Operating (default), FASB - Financing/IASB and Both</t>
-  </si>
-  <si>
     <t>Property should show correct property</t>
   </si>
   <si>
@@ -1732,6 +1720,15 @@
   </si>
   <si>
     <t>UICheckbox.VerifyCheckboxCheckedFalse</t>
+  </si>
+  <si>
+    <t>UIDropDown.ompareDropDownValue</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>UIScheduleTable.test</t>
   </si>
 </sst>
 </file>
@@ -2055,7 +2052,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="172">
+  <cellXfs count="180">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2485,7 +2482,25 @@
     <xf numFmtId="0" fontId="11" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="11" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3517,7 +3532,7 @@
         <v>203</v>
       </c>
       <c r="C20" s="154" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D20" s="122" t="s">
         <v>2</v>
@@ -3534,7 +3549,7 @@
         <v>204</v>
       </c>
       <c r="C21" s="154" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D21" s="122" t="s">
         <v>2</v>
@@ -3551,7 +3566,7 @@
         <v>205</v>
       </c>
       <c r="C22" s="154" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
     </row>
   </sheetData>
@@ -15872,10 +15887,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A52F28-3949-0E4C-AC35-967E0AD937B0}">
-  <dimension ref="A1:Z64"/>
+  <dimension ref="A1:Z61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C72" sqref="C72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16346,7 +16361,7 @@
       </c>
       <c r="B17" s="145"/>
       <c r="C17" s="146" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="D17" s="121" t="s">
         <v>478</v>
@@ -16382,7 +16397,7 @@
       </c>
       <c r="B18" s="145"/>
       <c r="C18" s="121" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="D18" s="121" t="s">
         <v>240</v>
@@ -16418,7 +16433,7 @@
       </c>
       <c r="B19" s="145"/>
       <c r="C19" s="121" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="D19" s="121" t="s">
         <v>78</v>
@@ -16454,7 +16469,7 @@
       </c>
       <c r="B20" s="145"/>
       <c r="C20" s="121" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="D20" s="121" t="s">
         <v>91</v>
@@ -16490,13 +16505,13 @@
       </c>
       <c r="B21" s="145"/>
       <c r="C21" s="148" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="D21" s="147" t="s">
         <v>272</v>
       </c>
       <c r="E21" s="149" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F21" s="147" t="s">
         <v>486</v>
@@ -16526,16 +16541,16 @@
       </c>
       <c r="B22" s="145"/>
       <c r="C22" s="167" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="D22" s="167" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="E22" s="168" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="F22" s="123" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="G22" s="169">
         <v>5</v>
@@ -16562,7 +16577,7 @@
       </c>
       <c r="B23" s="145"/>
       <c r="C23" s="146" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="D23" s="121" t="s">
         <v>235</v>
@@ -16596,7 +16611,7 @@
       </c>
       <c r="B24" s="145"/>
       <c r="C24" s="146" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="D24" s="121" t="s">
         <v>278</v>
@@ -16631,16 +16646,16 @@
         <v>119</v>
       </c>
       <c r="C25" s="146" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="D25" s="146" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="E25" s="150" t="s">
-        <v>95</v>
+        <v>561</v>
       </c>
       <c r="F25" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="G25" s="146" t="s">
         <v>151</v>
@@ -16662,31 +16677,30 @@
       <c r="P25" s="137"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="170">
-        <v>119</v>
-      </c>
-      <c r="C26" s="146" t="s">
-        <v>509</v>
-      </c>
-      <c r="D26" s="146" t="s">
+      <c r="A26" s="171"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="173" t="s">
+        <v>505</v>
+      </c>
+      <c r="D26" s="173" t="s">
+        <v>508</v>
+      </c>
+      <c r="E26" s="174" t="s">
+        <v>95</v>
+      </c>
+      <c r="F26" s="175" t="s">
         <v>512</v>
       </c>
-      <c r="E26" s="150" t="s">
-        <v>95</v>
-      </c>
-      <c r="F26" t="s">
-        <v>516</v>
-      </c>
-      <c r="G26" s="146" t="s">
-        <v>512</v>
-      </c>
-      <c r="H26" s="122" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J26" s="122" t="s">
+      <c r="G26" s="173" t="s">
+        <v>508</v>
+      </c>
+      <c r="H26" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="172" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="171" t="s">
         <v>12</v>
       </c>
       <c r="K26" s="137"/>
@@ -16697,31 +16711,30 @@
       <c r="P26" s="137"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="170">
-        <v>119</v>
-      </c>
-      <c r="C27" s="146" t="s">
-        <v>510</v>
-      </c>
-      <c r="D27" s="146" t="s">
-        <v>513</v>
-      </c>
-      <c r="E27" s="150" t="s">
+      <c r="A27" s="171"/>
+      <c r="B27" s="172"/>
+      <c r="C27" s="173" t="s">
+        <v>506</v>
+      </c>
+      <c r="D27" s="173" t="s">
+        <v>509</v>
+      </c>
+      <c r="E27" s="174" t="s">
         <v>95</v>
       </c>
-      <c r="F27" t="s">
-        <v>516</v>
-      </c>
-      <c r="G27" s="146" t="s">
-        <v>513</v>
-      </c>
-      <c r="H27" s="122" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J27" s="122" t="s">
+      <c r="F27" s="175" t="s">
+        <v>512</v>
+      </c>
+      <c r="G27" s="173" t="s">
+        <v>509</v>
+      </c>
+      <c r="H27" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="172" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="171" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="137"/>
@@ -16732,31 +16745,30 @@
       <c r="P27" s="137"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="170">
-        <v>119</v>
-      </c>
-      <c r="C28" s="146" t="s">
-        <v>508</v>
-      </c>
-      <c r="D28" s="146" t="s">
-        <v>511</v>
-      </c>
-      <c r="E28" s="150" t="s">
+      <c r="A28" s="171"/>
+      <c r="B28" s="172"/>
+      <c r="C28" s="173" t="s">
+        <v>504</v>
+      </c>
+      <c r="D28" s="173" t="s">
+        <v>507</v>
+      </c>
+      <c r="E28" s="174" t="s">
         <v>95</v>
       </c>
-      <c r="F28" t="s">
-        <v>516</v>
-      </c>
-      <c r="G28" s="146" t="s">
+      <c r="F28" s="175" t="s">
+        <v>512</v>
+      </c>
+      <c r="G28" s="173" t="s">
         <v>151</v>
       </c>
-      <c r="H28" s="122" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="J28" s="122" t="s">
+      <c r="H28" s="171" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="172" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="171" t="s">
         <v>12</v>
       </c>
       <c r="K28" s="137"/>
@@ -16767,24 +16779,30 @@
       <c r="P28" s="137"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C29" s="146" t="s">
-        <v>562</v>
-      </c>
-      <c r="D29" s="146" t="s">
-        <v>547</v>
-      </c>
-      <c r="E29" s="171" t="s">
-        <v>564</v>
-      </c>
-      <c r="F29" t="s">
-        <v>563</v>
-      </c>
+      <c r="A29" s="172"/>
+      <c r="B29" s="172"/>
+      <c r="C29" s="173" t="s">
+        <v>558</v>
+      </c>
+      <c r="D29" s="173" t="s">
+        <v>543</v>
+      </c>
+      <c r="E29" s="176" t="s">
+        <v>560</v>
+      </c>
+      <c r="F29" s="175" t="s">
+        <v>559</v>
+      </c>
+      <c r="G29" s="175"/>
+      <c r="H29" s="177"/>
+      <c r="I29" s="175"/>
+      <c r="J29" s="175"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A30" s="126"/>
       <c r="B30" s="126"/>
       <c r="C30" s="154" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="D30" s="123"/>
       <c r="E30" s="123"/>
@@ -16799,21 +16817,19 @@
         <v>203</v>
       </c>
       <c r="B31" s="15"/>
-      <c r="C31" s="152" t="s">
-        <v>517</v>
-      </c>
-      <c r="D31" s="150" t="s">
-        <v>518</v>
+      <c r="C31" s="178" t="s">
+        <v>562</v>
+      </c>
+      <c r="D31" s="179" t="s">
+        <v>562</v>
       </c>
       <c r="E31" s="15" t="s">
-        <v>546</v>
+        <v>563</v>
       </c>
       <c r="F31" s="153" t="s">
-        <v>519</v>
-      </c>
-      <c r="G31" s="153" t="s">
-        <v>520</v>
-      </c>
+        <v>515</v>
+      </c>
+      <c r="G31" s="15"/>
       <c r="H31" s="15" t="s">
         <v>12</v>
       </c>
@@ -16846,19 +16862,19 @@
       </c>
       <c r="B32" s="15"/>
       <c r="C32" s="152" t="s">
-        <v>521</v>
+        <v>513</v>
       </c>
       <c r="D32" s="150" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E32" s="15" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F32" s="153" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G32" s="153" t="s">
-        <v>522</v>
+        <v>516</v>
       </c>
       <c r="H32" s="15" t="s">
         <v>12</v>
@@ -16892,19 +16908,19 @@
       </c>
       <c r="B33" s="15"/>
       <c r="C33" s="152" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="D33" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E33" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F33" s="153" t="s">
+        <v>515</v>
+      </c>
+      <c r="G33" s="153" t="s">
         <v>518</v>
-      </c>
-      <c r="E33" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="F33" s="153" t="s">
-        <v>519</v>
-      </c>
-      <c r="G33" s="153" t="s">
-        <v>524</v>
       </c>
       <c r="H33" s="15" t="s">
         <v>12</v>
@@ -16938,19 +16954,19 @@
       </c>
       <c r="B34" s="15"/>
       <c r="C34" s="152" t="s">
-        <v>525</v>
+        <v>519</v>
       </c>
       <c r="D34" s="150" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E34" s="15" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F34" s="153" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="G34" s="153" t="s">
-        <v>526</v>
+        <v>520</v>
       </c>
       <c r="H34" s="15" t="s">
         <v>12</v>
@@ -16979,54 +16995,54 @@
       <c r="Z34" s="153"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C35" s="146"/>
+      <c r="A35" s="151">
+        <v>203</v>
+      </c>
+      <c r="B35" s="15"/>
+      <c r="C35" s="152" t="s">
+        <v>521</v>
+      </c>
+      <c r="D35" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F35" s="153" t="s">
+        <v>515</v>
+      </c>
+      <c r="G35" s="153" t="s">
+        <v>522</v>
+      </c>
+      <c r="H35" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I35" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J35" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
       <c r="C36" s="146"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="126"/>
-      <c r="B37" s="126"/>
-      <c r="C37" s="154" t="s">
-        <v>528</v>
-      </c>
-      <c r="D37" s="123"/>
-      <c r="E37" s="123"/>
-      <c r="F37" s="123"/>
-      <c r="G37" s="123"/>
-      <c r="H37" s="155"/>
-      <c r="I37" s="123"/>
-      <c r="J37" s="123"/>
+      <c r="C37" s="146"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="151">
-        <v>204</v>
-      </c>
-      <c r="B38" s="15"/>
-      <c r="C38" s="156" t="s">
-        <v>528</v>
-      </c>
-      <c r="D38" s="156" t="s">
-        <v>529</v>
-      </c>
-      <c r="E38" s="150" t="s">
-        <v>530</v>
-      </c>
-      <c r="F38" s="153" t="s">
-        <v>531</v>
-      </c>
-      <c r="G38" s="153" t="s">
-        <v>548</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I38" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J38" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="A38" s="126"/>
+      <c r="B38" s="126"/>
+      <c r="C38" s="154" t="s">
+        <v>524</v>
+      </c>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
+      <c r="F38" s="123"/>
+      <c r="G38" s="123"/>
+      <c r="H38" s="155"/>
+      <c r="I38" s="123"/>
+      <c r="J38" s="123"/>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -17048,21 +17064,20 @@
       <c r="A39" s="151">
         <v>204</v>
       </c>
-      <c r="C39" s="156" t="s">
-        <v>528</v>
-      </c>
-      <c r="D39" s="157" t="s">
-        <v>532</v>
-      </c>
-      <c r="E39" s="150" t="s">
-        <v>533</v>
+      <c r="B39" s="15"/>
+      <c r="C39" s="178" t="s">
+        <v>562</v>
+      </c>
+      <c r="D39" s="179" t="s">
+        <v>562</v>
+      </c>
+      <c r="E39" s="15" t="s">
+        <v>563</v>
       </c>
       <c r="F39" s="153" t="s">
-        <v>531</v>
-      </c>
-      <c r="G39" s="153" t="s">
-        <v>549</v>
-      </c>
+        <v>527</v>
+      </c>
+      <c r="G39" s="15"/>
       <c r="H39" s="15" t="s">
         <v>12</v>
       </c>
@@ -17095,19 +17110,19 @@
       </c>
       <c r="B40" s="15"/>
       <c r="C40" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D40" s="156" t="s">
-        <v>534</v>
+        <v>525</v>
       </c>
       <c r="E40" s="150" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="F40" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G40" s="153" t="s">
-        <v>550</v>
+        <v>544</v>
       </c>
       <c r="H40" s="15" t="s">
         <v>12</v>
@@ -17139,21 +17154,20 @@
       <c r="A41" s="151">
         <v>204</v>
       </c>
-      <c r="B41" s="15"/>
       <c r="C41" s="156" t="s">
+        <v>524</v>
+      </c>
+      <c r="D41" s="157" t="s">
         <v>528</v>
       </c>
-      <c r="D41" s="156" t="s">
-        <v>535</v>
-      </c>
       <c r="E41" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F41" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G41" s="153" t="s">
-        <v>551</v>
+        <v>545</v>
       </c>
       <c r="H41" s="15" t="s">
         <v>12</v>
@@ -17187,19 +17201,19 @@
       </c>
       <c r="B42" s="15"/>
       <c r="C42" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D42" s="156" t="s">
-        <v>536</v>
+        <v>530</v>
       </c>
       <c r="E42" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F42" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G42" s="153" t="s">
-        <v>552</v>
+        <v>546</v>
       </c>
       <c r="H42" s="15" t="s">
         <v>12</v>
@@ -17233,19 +17247,19 @@
       </c>
       <c r="B43" s="15"/>
       <c r="C43" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D43" s="156" t="s">
-        <v>537</v>
+        <v>531</v>
       </c>
       <c r="E43" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F43" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G43" s="153" t="s">
-        <v>553</v>
+        <v>547</v>
       </c>
       <c r="H43" s="15" t="s">
         <v>12</v>
@@ -17279,19 +17293,19 @@
       </c>
       <c r="B44" s="15"/>
       <c r="C44" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D44" s="156" t="s">
-        <v>538</v>
+        <v>532</v>
       </c>
       <c r="E44" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F44" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G44" s="153" t="s">
-        <v>554</v>
+        <v>548</v>
       </c>
       <c r="H44" s="15" t="s">
         <v>12</v>
@@ -17325,19 +17339,19 @@
       </c>
       <c r="B45" s="15"/>
       <c r="C45" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D45" s="156" t="s">
-        <v>539</v>
+        <v>533</v>
       </c>
       <c r="E45" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F45" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G45" s="153" t="s">
-        <v>555</v>
+        <v>549</v>
       </c>
       <c r="H45" s="15" t="s">
         <v>12</v>
@@ -17371,19 +17385,19 @@
       </c>
       <c r="B46" s="15"/>
       <c r="C46" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D46" s="156" t="s">
-        <v>540</v>
+        <v>534</v>
       </c>
       <c r="E46" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F46" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G46" s="153" t="s">
-        <v>556</v>
+        <v>550</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>12</v>
@@ -17417,19 +17431,19 @@
       </c>
       <c r="B47" s="15"/>
       <c r="C47" s="156" t="s">
-        <v>528</v>
-      </c>
-      <c r="D47" s="157" t="s">
-        <v>541</v>
+        <v>524</v>
+      </c>
+      <c r="D47" s="156" t="s">
+        <v>535</v>
       </c>
       <c r="E47" s="150" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="F47" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G47" s="153" t="s">
-        <v>557</v>
+        <v>551</v>
       </c>
       <c r="H47" s="15" t="s">
         <v>12</v>
@@ -17463,19 +17477,19 @@
       </c>
       <c r="B48" s="15"/>
       <c r="C48" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D48" s="156" t="s">
-        <v>542</v>
+        <v>536</v>
       </c>
       <c r="E48" s="150" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F48" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G48" s="153" t="s">
-        <v>558</v>
+        <v>552</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>12</v>
@@ -17509,19 +17523,19 @@
       </c>
       <c r="B49" s="15"/>
       <c r="C49" s="156" t="s">
-        <v>528</v>
-      </c>
-      <c r="D49" s="156" t="s">
-        <v>543</v>
+        <v>524</v>
+      </c>
+      <c r="D49" s="157" t="s">
+        <v>537</v>
       </c>
       <c r="E49" s="150" t="s">
-        <v>530</v>
+        <v>529</v>
       </c>
       <c r="F49" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G49" s="153" t="s">
-        <v>559</v>
+        <v>553</v>
       </c>
       <c r="H49" s="15" t="s">
         <v>12</v>
@@ -17555,19 +17569,19 @@
       </c>
       <c r="B50" s="15"/>
       <c r="C50" s="156" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="D50" s="156" t="s">
-        <v>560</v>
+        <v>538</v>
       </c>
       <c r="E50" s="150" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="F50" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G50" s="153" t="s">
-        <v>561</v>
+        <v>554</v>
       </c>
       <c r="H50" s="15" t="s">
         <v>12</v>
@@ -17596,97 +17610,97 @@
       <c r="Z50" s="153"/>
     </row>
     <row r="51" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C51" s="146"/>
+      <c r="A51" s="151">
+        <v>204</v>
+      </c>
+      <c r="B51" s="15"/>
+      <c r="C51" s="156" t="s">
+        <v>524</v>
+      </c>
+      <c r="D51" s="156" t="s">
+        <v>539</v>
+      </c>
+      <c r="E51" s="150" t="s">
+        <v>526</v>
+      </c>
+      <c r="F51" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G51" s="153" t="s">
+        <v>555</v>
+      </c>
+      <c r="H51" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I51" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J51" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K51" s="15"/>
+      <c r="L51" s="15"/>
+      <c r="M51" s="15"/>
+      <c r="N51" s="15"/>
+      <c r="O51" s="153"/>
+      <c r="P51" s="153"/>
+      <c r="Q51" s="153"/>
+      <c r="R51" s="153"/>
+      <c r="S51" s="153"/>
+      <c r="T51" s="153"/>
+      <c r="U51" s="153"/>
+      <c r="V51" s="153"/>
+      <c r="W51" s="153"/>
+      <c r="X51" s="153"/>
+      <c r="Y51" s="153"/>
+      <c r="Z51" s="153"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="126"/>
-      <c r="B52" s="126"/>
-      <c r="C52" s="154" t="s">
-        <v>544</v>
-      </c>
-      <c r="D52" s="123"/>
-      <c r="E52" s="123"/>
-      <c r="F52" s="123"/>
-      <c r="G52" s="123"/>
-      <c r="H52" s="155"/>
-      <c r="I52" s="123"/>
-      <c r="J52" s="123"/>
+      <c r="A52" s="151">
+        <v>204</v>
+      </c>
+      <c r="B52" s="15"/>
+      <c r="C52" s="156" t="s">
+        <v>524</v>
+      </c>
+      <c r="D52" s="156" t="s">
+        <v>556</v>
+      </c>
+      <c r="E52" s="150" t="s">
+        <v>526</v>
+      </c>
+      <c r="F52" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G52" s="153" t="s">
+        <v>557</v>
+      </c>
+      <c r="H52" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I52" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J52" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A53" s="151">
-        <v>205</v>
-      </c>
-      <c r="B53" s="15"/>
-      <c r="C53" s="152" t="s">
-        <v>517</v>
-      </c>
-      <c r="D53" s="150" t="s">
-        <v>518</v>
-      </c>
-      <c r="E53" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="F53" s="153" t="s">
-        <v>531</v>
-      </c>
-      <c r="G53" s="153" t="s">
-        <v>520</v>
-      </c>
-      <c r="H53" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I53" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J53" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="153"/>
-      <c r="P53" s="153"/>
-      <c r="Q53" s="153"/>
-      <c r="R53" s="153"/>
-      <c r="S53" s="153"/>
-      <c r="T53" s="153"/>
-      <c r="U53" s="153"/>
-      <c r="V53" s="153"/>
-      <c r="W53" s="153"/>
-      <c r="X53" s="153"/>
-      <c r="Y53" s="153"/>
-      <c r="Z53" s="153"/>
+      <c r="C53" s="146"/>
     </row>
     <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="151">
-        <v>205</v>
-      </c>
-      <c r="B54" s="15"/>
-      <c r="C54" s="152" t="s">
-        <v>521</v>
-      </c>
-      <c r="D54" s="150" t="s">
-        <v>518</v>
-      </c>
-      <c r="E54" s="15" t="s">
-        <v>546</v>
-      </c>
-      <c r="F54" s="153" t="s">
-        <v>531</v>
-      </c>
-      <c r="G54" s="153" t="s">
-        <v>522</v>
-      </c>
-      <c r="H54" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I54" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J54" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="A54" s="126"/>
+      <c r="B54" s="126"/>
+      <c r="C54" s="154" t="s">
+        <v>540</v>
+      </c>
+      <c r="D54" s="123"/>
+      <c r="E54" s="123"/>
+      <c r="F54" s="123"/>
+      <c r="G54" s="123"/>
+      <c r="H54" s="155"/>
+      <c r="I54" s="123"/>
+      <c r="J54" s="123"/>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -17708,22 +17722,20 @@
       <c r="A55" s="151">
         <v>205</v>
       </c>
-      <c r="B55" s="15"/>
-      <c r="C55" s="152" t="s">
-        <v>523</v>
-      </c>
-      <c r="D55" s="150" t="s">
-        <v>518</v>
+      <c r="B55" s="126"/>
+      <c r="C55" s="178" t="s">
+        <v>562</v>
+      </c>
+      <c r="D55" s="179" t="s">
+        <v>562</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>546</v>
+        <v>563</v>
       </c>
       <c r="F55" s="153" t="s">
-        <v>531</v>
-      </c>
-      <c r="G55" s="153" t="s">
-        <v>524</v>
-      </c>
+        <v>527</v>
+      </c>
+      <c r="G55" s="15"/>
       <c r="H55" s="15" t="s">
         <v>12</v>
       </c>
@@ -17756,19 +17768,19 @@
       </c>
       <c r="B56" s="15"/>
       <c r="C56" s="152" t="s">
-        <v>525</v>
+        <v>513</v>
       </c>
       <c r="D56" s="150" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="E56" s="15" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="F56" s="153" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="G56" s="153" t="s">
-        <v>526</v>
+        <v>516</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>12</v>
@@ -17796,28 +17808,130 @@
       <c r="Y56" s="153"/>
       <c r="Z56" s="153"/>
     </row>
+    <row r="57" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A57" s="151">
+        <v>205</v>
+      </c>
+      <c r="B57" s="15"/>
+      <c r="C57" s="152" t="s">
+        <v>517</v>
+      </c>
+      <c r="D57" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E57" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F57" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G57" s="153" t="s">
+        <v>518</v>
+      </c>
+      <c r="H57" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I57" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J57" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K57" s="15"/>
+      <c r="L57" s="15"/>
+      <c r="M57" s="15"/>
+      <c r="N57" s="15"/>
+      <c r="O57" s="153"/>
+      <c r="P57" s="153"/>
+      <c r="Q57" s="153"/>
+      <c r="R57" s="153"/>
+      <c r="S57" s="153"/>
+      <c r="T57" s="153"/>
+      <c r="U57" s="153"/>
+      <c r="V57" s="153"/>
+      <c r="W57" s="153"/>
+      <c r="X57" s="153"/>
+      <c r="Y57" s="153"/>
+      <c r="Z57" s="153"/>
+    </row>
     <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C58" s="146"/>
+      <c r="A58" s="151">
+        <v>205</v>
+      </c>
+      <c r="B58" s="15"/>
+      <c r="C58" s="152" t="s">
+        <v>519</v>
+      </c>
+      <c r="D58" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E58" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F58" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G58" s="153" t="s">
+        <v>520</v>
+      </c>
+      <c r="H58" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I58" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J58" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="K58" s="15"/>
+      <c r="L58" s="15"/>
+      <c r="M58" s="15"/>
+      <c r="N58" s="15"/>
+      <c r="O58" s="153"/>
+      <c r="P58" s="153"/>
+      <c r="Q58" s="153"/>
+      <c r="R58" s="153"/>
+      <c r="S58" s="153"/>
+      <c r="T58" s="153"/>
+      <c r="U58" s="153"/>
+      <c r="V58" s="153"/>
+      <c r="W58" s="153"/>
+      <c r="X58" s="153"/>
+      <c r="Y58" s="153"/>
+      <c r="Z58" s="153"/>
+    </row>
+    <row r="59" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A59" s="151">
+        <v>205</v>
+      </c>
+      <c r="B59" s="15"/>
+      <c r="C59" s="152" t="s">
+        <v>521</v>
+      </c>
+      <c r="D59" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E59" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F59" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G59" s="153" t="s">
+        <v>522</v>
+      </c>
+      <c r="H59" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I59" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J59" s="15" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C61" s="146" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="62" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C62" s="146" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="63" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C63" s="146" t="s">
-        <v>498</v>
-      </c>
-    </row>
-    <row r="64" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C64" s="146" t="s">
-        <v>499</v>
-      </c>
+      <c r="C61" s="146"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
checkPeriodPayment and paymentPeriodTest method added
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84399283-AF0B-804C-9E88-237921DA1EDB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E48ADFD-7FAC-6D45-BCEE-40E802B63CFF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3308" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3294" uniqueCount="564">
   <si>
     <t>Action</t>
   </si>
@@ -2052,7 +2052,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="184">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2450,30 +2450,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2503,6 +2479,38 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Accent1" xfId="2" builtinId="29"/>
@@ -3579,7 +3587,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L389"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView topLeftCell="A118" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="C192" sqref="C192"/>
     </sheetView>
   </sheetViews>
@@ -3637,16 +3645,16 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
-      <c r="C2" s="162" t="s">
+      <c r="C2" s="176" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="162"/>
-      <c r="E2" s="162"/>
-      <c r="F2" s="162"/>
-      <c r="G2" s="162"/>
-      <c r="H2" s="162"/>
-      <c r="I2" s="162"/>
-      <c r="J2" s="162"/>
+      <c r="D2" s="176"/>
+      <c r="E2" s="176"/>
+      <c r="F2" s="176"/>
+      <c r="G2" s="176"/>
+      <c r="H2" s="176"/>
+      <c r="I2" s="176"/>
+      <c r="J2" s="176"/>
       <c r="K2" s="32"/>
       <c r="L2" s="33"/>
     </row>
@@ -4789,16 +4797,16 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
       <c r="B39" s="32"/>
-      <c r="C39" s="162" t="s">
+      <c r="C39" s="176" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="162"/>
-      <c r="E39" s="162"/>
-      <c r="F39" s="162"/>
-      <c r="G39" s="162"/>
-      <c r="H39" s="162"/>
-      <c r="I39" s="162"/>
-      <c r="J39" s="162"/>
+      <c r="D39" s="176"/>
+      <c r="E39" s="176"/>
+      <c r="F39" s="176"/>
+      <c r="G39" s="176"/>
+      <c r="H39" s="176"/>
+      <c r="I39" s="176"/>
+      <c r="J39" s="176"/>
       <c r="K39" s="32"/>
       <c r="L39" s="33"/>
     </row>
@@ -6032,16 +6040,16 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="31"/>
       <c r="B79" s="32"/>
-      <c r="C79" s="162" t="s">
+      <c r="C79" s="176" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="162"/>
-      <c r="E79" s="162"/>
-      <c r="F79" s="162"/>
-      <c r="G79" s="162"/>
-      <c r="H79" s="162"/>
-      <c r="I79" s="162"/>
-      <c r="J79" s="162"/>
+      <c r="D79" s="176"/>
+      <c r="E79" s="176"/>
+      <c r="F79" s="176"/>
+      <c r="G79" s="176"/>
+      <c r="H79" s="176"/>
+      <c r="I79" s="176"/>
+      <c r="J79" s="176"/>
       <c r="K79" s="32"/>
       <c r="L79" s="33"/>
     </row>
@@ -7432,16 +7440,16 @@
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="31"/>
       <c r="B126" s="32"/>
-      <c r="C126" s="162" t="s">
+      <c r="C126" s="176" t="s">
         <v>198</v>
       </c>
-      <c r="D126" s="162"/>
-      <c r="E126" s="162"/>
-      <c r="F126" s="162"/>
-      <c r="G126" s="162"/>
-      <c r="H126" s="162"/>
-      <c r="I126" s="162"/>
-      <c r="J126" s="162"/>
+      <c r="D126" s="176"/>
+      <c r="E126" s="176"/>
+      <c r="F126" s="176"/>
+      <c r="G126" s="176"/>
+      <c r="H126" s="176"/>
+      <c r="I126" s="176"/>
+      <c r="J126" s="176"/>
       <c r="K126" s="32"/>
       <c r="L126" s="33"/>
     </row>
@@ -8783,11 +8791,11 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="163" t="s">
+      <c r="B170" s="177" t="s">
         <v>206</v>
       </c>
-      <c r="C170" s="163"/>
-      <c r="D170" s="163"/>
+      <c r="C170" s="177"/>
+      <c r="D170" s="177"/>
       <c r="H170" s="75"/>
     </row>
     <row r="171" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -9296,11 +9304,11 @@
       <c r="J186" s="18"/>
     </row>
     <row r="187" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B187" s="160" t="s">
+      <c r="B187" s="172" t="s">
         <v>211</v>
       </c>
-      <c r="C187" s="160"/>
-      <c r="D187" s="160"/>
+      <c r="C187" s="172"/>
+      <c r="D187" s="172"/>
       <c r="H187" s="83"/>
     </row>
     <row r="188" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -9619,11 +9627,11 @@
       </c>
     </row>
     <row r="201" spans="1:12" s="87" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="164" t="s">
+      <c r="B201" s="173" t="s">
         <v>202</v>
       </c>
-      <c r="C201" s="164"/>
-      <c r="D201" s="164"/>
+      <c r="C201" s="173"/>
+      <c r="D201" s="173"/>
       <c r="H201" s="88"/>
     </row>
     <row r="202" spans="1:12" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -10179,11 +10187,11 @@
       </c>
     </row>
     <row r="220" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B220" s="165" t="s">
+      <c r="B220" s="174" t="s">
         <v>203</v>
       </c>
-      <c r="C220" s="165"/>
-      <c r="D220" s="165"/>
+      <c r="C220" s="174"/>
+      <c r="D220" s="174"/>
       <c r="H220" s="75"/>
     </row>
     <row r="221" spans="1:12" s="95" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -11240,11 +11248,11 @@
       </c>
     </row>
     <row r="254" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B254" s="166" t="s">
+      <c r="B254" s="175" t="s">
         <v>204</v>
       </c>
-      <c r="C254" s="166"/>
-      <c r="D254" s="166"/>
+      <c r="C254" s="175"/>
+      <c r="D254" s="175"/>
       <c r="H254" s="83"/>
     </row>
     <row r="255" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -11622,11 +11630,11 @@
       </c>
     </row>
     <row r="267" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B267" s="166" t="s">
+      <c r="B267" s="175" t="s">
         <v>205</v>
       </c>
-      <c r="C267" s="166"/>
-      <c r="D267" s="166"/>
+      <c r="C267" s="175"/>
+      <c r="D267" s="175"/>
       <c r="H267" s="83"/>
     </row>
     <row r="268" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -12342,11 +12350,11 @@
       </c>
     </row>
     <row r="291" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B291" s="160" t="s">
+      <c r="B291" s="172" t="s">
         <v>415</v>
       </c>
-      <c r="C291" s="160"/>
-      <c r="D291" s="160"/>
+      <c r="C291" s="172"/>
+      <c r="D291" s="172"/>
       <c r="H291" s="83"/>
     </row>
     <row r="292" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -12646,11 +12654,11 @@
       </c>
     </row>
     <row r="301" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B301" s="161" t="s">
+      <c r="B301" s="179" t="s">
         <v>414</v>
       </c>
-      <c r="C301" s="161"/>
-      <c r="D301" s="161"/>
+      <c r="C301" s="179"/>
+      <c r="D301" s="179"/>
       <c r="H301" s="83"/>
     </row>
     <row r="302" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -12917,12 +12925,12 @@
     </row>
     <row r="310" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A310" s="111"/>
-      <c r="B310" s="159" t="s">
+      <c r="B310" s="178" t="s">
         <v>424</v>
       </c>
-      <c r="C310" s="159"/>
-      <c r="D310" s="159"/>
-      <c r="E310" s="159"/>
+      <c r="C310" s="178"/>
+      <c r="D310" s="178"/>
+      <c r="E310" s="178"/>
       <c r="F310" s="111"/>
       <c r="G310" s="111"/>
       <c r="H310" s="112"/>
@@ -13435,12 +13443,12 @@
     </row>
     <row r="328" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A328" s="111"/>
-      <c r="B328" s="159" t="s">
+      <c r="B328" s="178" t="s">
         <v>440</v>
       </c>
-      <c r="C328" s="159"/>
-      <c r="D328" s="159"/>
-      <c r="E328" s="159"/>
+      <c r="C328" s="178"/>
+      <c r="D328" s="178"/>
+      <c r="E328" s="178"/>
       <c r="F328" s="111"/>
       <c r="G328" s="111"/>
       <c r="H328" s="112"/>
@@ -14443,12 +14451,12 @@
     </row>
     <row r="360" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A360" s="111"/>
-      <c r="B360" s="159" t="s">
+      <c r="B360" s="178" t="s">
         <v>442</v>
       </c>
-      <c r="C360" s="159"/>
-      <c r="D360" s="159"/>
-      <c r="E360" s="159"/>
+      <c r="C360" s="178"/>
+      <c r="D360" s="178"/>
+      <c r="E360" s="178"/>
       <c r="F360" s="111"/>
       <c r="G360" s="111"/>
       <c r="H360" s="112"/>
@@ -14930,12 +14938,12 @@
     </row>
     <row r="375" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A375" s="111"/>
-      <c r="B375" s="159" t="s">
+      <c r="B375" s="178" t="s">
         <v>462</v>
       </c>
-      <c r="C375" s="159"/>
-      <c r="D375" s="159"/>
-      <c r="E375" s="159"/>
+      <c r="C375" s="178"/>
+      <c r="D375" s="178"/>
+      <c r="E375" s="178"/>
       <c r="F375" s="111"/>
       <c r="G375" s="111"/>
       <c r="H375" s="112"/>
@@ -15150,12 +15158,12 @@
     </row>
     <row r="383" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A383" s="111"/>
-      <c r="B383" s="159" t="s">
+      <c r="B383" s="178" t="s">
         <v>463</v>
       </c>
-      <c r="C383" s="159"/>
-      <c r="D383" s="159"/>
-      <c r="E383" s="159"/>
+      <c r="C383" s="178"/>
+      <c r="D383" s="178"/>
+      <c r="E383" s="178"/>
       <c r="F383" s="111"/>
       <c r="G383" s="111"/>
       <c r="H383" s="112"/>
@@ -15370,16 +15378,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B187:D187"/>
-    <mergeCell ref="B201:D201"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="B254:D254"/>
-    <mergeCell ref="B267:D267"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C126:J126"/>
-    <mergeCell ref="B170:D170"/>
     <mergeCell ref="B360:E360"/>
     <mergeCell ref="B291:D291"/>
     <mergeCell ref="B301:D301"/>
@@ -15387,6 +15385,16 @@
     <mergeCell ref="B383:E383"/>
     <mergeCell ref="B310:E310"/>
     <mergeCell ref="B328:E328"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C126:J126"/>
+    <mergeCell ref="B170:D170"/>
+    <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B201:D201"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="B254:D254"/>
+    <mergeCell ref="B267:D267"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="43" priority="425" operator="equal">
@@ -15887,10 +15895,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A52F28-3949-0E4C-AC35-967E0AD937B0}">
-  <dimension ref="A1:Z61"/>
+  <dimension ref="A1:Z59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C72" sqref="C72"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16356,7 +16364,7 @@
       <c r="L16" s="126"/>
     </row>
     <row r="17" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="170">
+      <c r="A17" s="162">
         <v>119</v>
       </c>
       <c r="B17" s="145"/>
@@ -16392,7 +16400,7 @@
       <c r="P17" s="137"/>
     </row>
     <row r="18" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="170">
+      <c r="A18" s="162">
         <v>119</v>
       </c>
       <c r="B18" s="145"/>
@@ -16428,7 +16436,7 @@
       <c r="P18" s="137"/>
     </row>
     <row r="19" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="170">
+      <c r="A19" s="162">
         <v>119</v>
       </c>
       <c r="B19" s="145"/>
@@ -16464,7 +16472,7 @@
       <c r="P19" s="137"/>
     </row>
     <row r="20" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="170">
+      <c r="A20" s="162">
         <v>119</v>
       </c>
       <c r="B20" s="145"/>
@@ -16500,7 +16508,7 @@
       <c r="P20" s="137"/>
     </row>
     <row r="21" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="170">
+      <c r="A21" s="162">
         <v>119</v>
       </c>
       <c r="B21" s="145"/>
@@ -16536,23 +16544,23 @@
       <c r="P21" s="137"/>
     </row>
     <row r="22" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="170">
+      <c r="A22" s="162">
         <v>119</v>
       </c>
       <c r="B22" s="145"/>
-      <c r="C22" s="167" t="s">
+      <c r="C22" s="159" t="s">
         <v>501</v>
       </c>
-      <c r="D22" s="167" t="s">
+      <c r="D22" s="159" t="s">
         <v>511</v>
       </c>
-      <c r="E22" s="168" t="s">
+      <c r="E22" s="160" t="s">
         <v>541</v>
       </c>
       <c r="F22" s="123" t="s">
         <v>510</v>
       </c>
-      <c r="G22" s="169">
+      <c r="G22" s="161">
         <v>5</v>
       </c>
       <c r="H22" s="122" t="s">
@@ -16572,7 +16580,7 @@
       <c r="P22" s="137"/>
     </row>
     <row r="23" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="170">
+      <c r="A23" s="162">
         <v>119</v>
       </c>
       <c r="B23" s="145"/>
@@ -16606,7 +16614,7 @@
       <c r="P23" s="137"/>
     </row>
     <row r="24" spans="1:26" s="123" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="170">
+      <c r="A24" s="162">
         <v>119</v>
       </c>
       <c r="B24" s="145"/>
@@ -16642,9 +16650,7 @@
       <c r="P24" s="137"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="170">
-        <v>119</v>
-      </c>
+      <c r="A25" s="162"/>
       <c r="C25" s="146" t="s">
         <v>504</v>
       </c>
@@ -16677,30 +16683,30 @@
       <c r="P25" s="137"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="171"/>
-      <c r="B26" s="172"/>
-      <c r="C26" s="173" t="s">
+      <c r="A26" s="163"/>
+      <c r="B26" s="164"/>
+      <c r="C26" s="165" t="s">
         <v>505</v>
       </c>
-      <c r="D26" s="173" t="s">
+      <c r="D26" s="165" t="s">
         <v>508</v>
       </c>
-      <c r="E26" s="174" t="s">
+      <c r="E26" s="166" t="s">
         <v>95</v>
       </c>
-      <c r="F26" s="175" t="s">
+      <c r="F26" s="167" t="s">
         <v>512</v>
       </c>
-      <c r="G26" s="173" t="s">
+      <c r="G26" s="165" t="s">
         <v>508</v>
       </c>
-      <c r="H26" s="171" t="s">
-        <v>12</v>
-      </c>
-      <c r="I26" s="172" t="s">
-        <v>2</v>
-      </c>
-      <c r="J26" s="171" t="s">
+      <c r="H26" s="163" t="s">
+        <v>12</v>
+      </c>
+      <c r="I26" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" s="163" t="s">
         <v>12</v>
       </c>
       <c r="K26" s="137"/>
@@ -16711,30 +16717,30 @@
       <c r="P26" s="137"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="171"/>
-      <c r="B27" s="172"/>
-      <c r="C27" s="173" t="s">
+      <c r="A27" s="163"/>
+      <c r="B27" s="164"/>
+      <c r="C27" s="165" t="s">
         <v>506</v>
       </c>
-      <c r="D27" s="173" t="s">
+      <c r="D27" s="165" t="s">
         <v>509</v>
       </c>
-      <c r="E27" s="174" t="s">
+      <c r="E27" s="166" t="s">
         <v>95</v>
       </c>
-      <c r="F27" s="175" t="s">
+      <c r="F27" s="167" t="s">
         <v>512</v>
       </c>
-      <c r="G27" s="173" t="s">
+      <c r="G27" s="165" t="s">
         <v>509</v>
       </c>
-      <c r="H27" s="171" t="s">
-        <v>12</v>
-      </c>
-      <c r="I27" s="172" t="s">
-        <v>2</v>
-      </c>
-      <c r="J27" s="171" t="s">
+      <c r="H27" s="163" t="s">
+        <v>12</v>
+      </c>
+      <c r="I27" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="J27" s="163" t="s">
         <v>12</v>
       </c>
       <c r="K27" s="137"/>
@@ -16745,30 +16751,30 @@
       <c r="P27" s="137"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="171"/>
-      <c r="B28" s="172"/>
-      <c r="C28" s="173" t="s">
+      <c r="A28" s="163"/>
+      <c r="B28" s="164"/>
+      <c r="C28" s="165" t="s">
         <v>504</v>
       </c>
-      <c r="D28" s="173" t="s">
+      <c r="D28" s="165" t="s">
         <v>507</v>
       </c>
-      <c r="E28" s="174" t="s">
+      <c r="E28" s="166" t="s">
         <v>95</v>
       </c>
-      <c r="F28" s="175" t="s">
+      <c r="F28" s="167" t="s">
         <v>512</v>
       </c>
-      <c r="G28" s="173" t="s">
+      <c r="G28" s="165" t="s">
         <v>151</v>
       </c>
-      <c r="H28" s="171" t="s">
-        <v>12</v>
-      </c>
-      <c r="I28" s="172" t="s">
-        <v>2</v>
-      </c>
-      <c r="J28" s="171" t="s">
+      <c r="H28" s="163" t="s">
+        <v>12</v>
+      </c>
+      <c r="I28" s="164" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="163" t="s">
         <v>12</v>
       </c>
       <c r="K28" s="137"/>
@@ -16779,82 +16785,49 @@
       <c r="P28" s="137"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="172"/>
-      <c r="B29" s="172"/>
-      <c r="C29" s="173" t="s">
+      <c r="A29" s="162">
+        <v>119</v>
+      </c>
+      <c r="B29" s="164"/>
+      <c r="C29" s="165" t="s">
         <v>558</v>
       </c>
-      <c r="D29" s="173" t="s">
+      <c r="D29" s="165" t="s">
         <v>543</v>
       </c>
-      <c r="E29" s="176" t="s">
+      <c r="E29" s="168" t="s">
         <v>560</v>
       </c>
-      <c r="F29" s="175" t="s">
+      <c r="F29" s="167" t="s">
         <v>559</v>
       </c>
-      <c r="G29" s="175"/>
-      <c r="H29" s="177"/>
-      <c r="I29" s="175"/>
-      <c r="J29" s="175"/>
-    </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="126"/>
-      <c r="B30" s="126"/>
-      <c r="C30" s="154" t="s">
+      <c r="G29" s="167"/>
+      <c r="H29" s="169"/>
+      <c r="I29" s="167"/>
+      <c r="J29" s="167"/>
+    </row>
+    <row r="30" spans="1:26" s="136" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="180"/>
+      <c r="B30" s="180"/>
+      <c r="C30" s="181"/>
+      <c r="D30" s="181"/>
+      <c r="E30" s="182"/>
+      <c r="H30" s="183"/>
+      <c r="L30" s="180"/>
+    </row>
+    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A31" s="126"/>
+      <c r="B31" s="126"/>
+      <c r="C31" s="154" t="s">
         <v>523</v>
       </c>
-      <c r="D30" s="123"/>
-      <c r="E30" s="123"/>
-      <c r="F30" s="123"/>
-      <c r="G30" s="123"/>
-      <c r="H30" s="155"/>
-      <c r="I30" s="123"/>
-      <c r="J30" s="123"/>
-    </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="151">
-        <v>203</v>
-      </c>
-      <c r="B31" s="15"/>
-      <c r="C31" s="178" t="s">
-        <v>562</v>
-      </c>
-      <c r="D31" s="179" t="s">
-        <v>562</v>
-      </c>
-      <c r="E31" s="15" t="s">
-        <v>563</v>
-      </c>
-      <c r="F31" s="153" t="s">
-        <v>515</v>
-      </c>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J31" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="153"/>
-      <c r="P31" s="153"/>
-      <c r="Q31" s="153"/>
-      <c r="R31" s="153"/>
-      <c r="S31" s="153"/>
-      <c r="T31" s="153"/>
-      <c r="U31" s="153"/>
-      <c r="V31" s="153"/>
-      <c r="W31" s="153"/>
-      <c r="X31" s="153"/>
-      <c r="Y31" s="153"/>
-      <c r="Z31" s="153"/>
+      <c r="D31" s="123"/>
+      <c r="E31" s="123"/>
+      <c r="F31" s="123"/>
+      <c r="G31" s="123"/>
+      <c r="H31" s="155"/>
+      <c r="I31" s="123"/>
+      <c r="J31" s="123"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A32" s="151">
@@ -17028,21 +17001,62 @@
       <c r="C36" s="146"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C37" s="146"/>
+      <c r="A37" s="126"/>
+      <c r="B37" s="126"/>
+      <c r="C37" s="154" t="s">
+        <v>524</v>
+      </c>
+      <c r="D37" s="123"/>
+      <c r="E37" s="123"/>
+      <c r="F37" s="123"/>
+      <c r="G37" s="123"/>
+      <c r="H37" s="155"/>
+      <c r="I37" s="123"/>
+      <c r="J37" s="123"/>
+      <c r="K37" s="15"/>
+      <c r="L37" s="15"/>
+      <c r="M37" s="15"/>
+      <c r="N37" s="15"/>
+      <c r="O37" s="153"/>
+      <c r="P37" s="153"/>
+      <c r="Q37" s="153"/>
+      <c r="R37" s="153"/>
+      <c r="S37" s="153"/>
+      <c r="T37" s="153"/>
+      <c r="U37" s="153"/>
+      <c r="V37" s="153"/>
+      <c r="W37" s="153"/>
+      <c r="X37" s="153"/>
+      <c r="Y37" s="153"/>
+      <c r="Z37" s="153"/>
     </row>
     <row r="38" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A38" s="126"/>
-      <c r="B38" s="126"/>
-      <c r="C38" s="154" t="s">
-        <v>524</v>
-      </c>
-      <c r="D38" s="123"/>
-      <c r="E38" s="123"/>
-      <c r="F38" s="123"/>
-      <c r="G38" s="123"/>
-      <c r="H38" s="155"/>
-      <c r="I38" s="123"/>
-      <c r="J38" s="123"/>
+      <c r="A38" s="151">
+        <v>204</v>
+      </c>
+      <c r="B38" s="15"/>
+      <c r="C38" s="170" t="s">
+        <v>562</v>
+      </c>
+      <c r="D38" s="171" t="s">
+        <v>562</v>
+      </c>
+      <c r="E38" s="15" t="s">
+        <v>563</v>
+      </c>
+      <c r="F38" s="153" t="s">
+        <v>527</v>
+      </c>
+      <c r="G38" s="15"/>
+      <c r="H38" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J38" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="K38" s="15"/>
       <c r="L38" s="15"/>
       <c r="M38" s="15"/>
@@ -17065,19 +17079,21 @@
         <v>204</v>
       </c>
       <c r="B39" s="15"/>
-      <c r="C39" s="178" t="s">
-        <v>562</v>
-      </c>
-      <c r="D39" s="179" t="s">
-        <v>562</v>
-      </c>
-      <c r="E39" s="15" t="s">
-        <v>563</v>
+      <c r="C39" s="156" t="s">
+        <v>524</v>
+      </c>
+      <c r="D39" s="156" t="s">
+        <v>525</v>
+      </c>
+      <c r="E39" s="150" t="s">
+        <v>526</v>
       </c>
       <c r="F39" s="153" t="s">
         <v>527</v>
       </c>
-      <c r="G39" s="15"/>
+      <c r="G39" s="153" t="s">
+        <v>544</v>
+      </c>
       <c r="H39" s="15" t="s">
         <v>12</v>
       </c>
@@ -17108,21 +17124,20 @@
       <c r="A40" s="151">
         <v>204</v>
       </c>
-      <c r="B40" s="15"/>
       <c r="C40" s="156" t="s">
         <v>524</v>
       </c>
-      <c r="D40" s="156" t="s">
-        <v>525</v>
+      <c r="D40" s="157" t="s">
+        <v>528</v>
       </c>
       <c r="E40" s="150" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="F40" s="153" t="s">
         <v>527</v>
       </c>
       <c r="G40" s="153" t="s">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="H40" s="15" t="s">
         <v>12</v>
@@ -17154,11 +17169,12 @@
       <c r="A41" s="151">
         <v>204</v>
       </c>
+      <c r="B41" s="15"/>
       <c r="C41" s="156" t="s">
         <v>524</v>
       </c>
-      <c r="D41" s="157" t="s">
-        <v>528</v>
+      <c r="D41" s="156" t="s">
+        <v>530</v>
       </c>
       <c r="E41" s="150" t="s">
         <v>529</v>
@@ -17167,7 +17183,7 @@
         <v>527</v>
       </c>
       <c r="G41" s="153" t="s">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="H41" s="15" t="s">
         <v>12</v>
@@ -17204,7 +17220,7 @@
         <v>524</v>
       </c>
       <c r="D42" s="156" t="s">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="E42" s="150" t="s">
         <v>529</v>
@@ -17213,7 +17229,7 @@
         <v>527</v>
       </c>
       <c r="G42" s="153" t="s">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="H42" s="15" t="s">
         <v>12</v>
@@ -17250,7 +17266,7 @@
         <v>524</v>
       </c>
       <c r="D43" s="156" t="s">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="E43" s="150" t="s">
         <v>529</v>
@@ -17259,7 +17275,7 @@
         <v>527</v>
       </c>
       <c r="G43" s="153" t="s">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="H43" s="15" t="s">
         <v>12</v>
@@ -17296,7 +17312,7 @@
         <v>524</v>
       </c>
       <c r="D44" s="156" t="s">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="E44" s="150" t="s">
         <v>529</v>
@@ -17305,7 +17321,7 @@
         <v>527</v>
       </c>
       <c r="G44" s="153" t="s">
-        <v>548</v>
+        <v>549</v>
       </c>
       <c r="H44" s="15" t="s">
         <v>12</v>
@@ -17342,7 +17358,7 @@
         <v>524</v>
       </c>
       <c r="D45" s="156" t="s">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="E45" s="150" t="s">
         <v>529</v>
@@ -17351,7 +17367,7 @@
         <v>527</v>
       </c>
       <c r="G45" s="153" t="s">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="H45" s="15" t="s">
         <v>12</v>
@@ -17388,7 +17404,7 @@
         <v>524</v>
       </c>
       <c r="D46" s="156" t="s">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="E46" s="150" t="s">
         <v>529</v>
@@ -17397,7 +17413,7 @@
         <v>527</v>
       </c>
       <c r="G46" s="153" t="s">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="H46" s="15" t="s">
         <v>12</v>
@@ -17434,7 +17450,7 @@
         <v>524</v>
       </c>
       <c r="D47" s="156" t="s">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="E47" s="150" t="s">
         <v>529</v>
@@ -17443,7 +17459,7 @@
         <v>527</v>
       </c>
       <c r="G47" s="153" t="s">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="H47" s="15" t="s">
         <v>12</v>
@@ -17479,8 +17495,8 @@
       <c r="C48" s="156" t="s">
         <v>524</v>
       </c>
-      <c r="D48" s="156" t="s">
-        <v>536</v>
+      <c r="D48" s="157" t="s">
+        <v>537</v>
       </c>
       <c r="E48" s="150" t="s">
         <v>529</v>
@@ -17489,7 +17505,7 @@
         <v>527</v>
       </c>
       <c r="G48" s="153" t="s">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="H48" s="15" t="s">
         <v>12</v>
@@ -17525,17 +17541,17 @@
       <c r="C49" s="156" t="s">
         <v>524</v>
       </c>
-      <c r="D49" s="157" t="s">
-        <v>537</v>
+      <c r="D49" s="156" t="s">
+        <v>538</v>
       </c>
       <c r="E49" s="150" t="s">
-        <v>529</v>
+        <v>526</v>
       </c>
       <c r="F49" s="153" t="s">
         <v>527</v>
       </c>
       <c r="G49" s="153" t="s">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="H49" s="15" t="s">
         <v>12</v>
@@ -17572,7 +17588,7 @@
         <v>524</v>
       </c>
       <c r="D50" s="156" t="s">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="E50" s="150" t="s">
         <v>526</v>
@@ -17581,7 +17597,7 @@
         <v>527</v>
       </c>
       <c r="G50" s="153" t="s">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="H50" s="15" t="s">
         <v>12</v>
@@ -17618,7 +17634,7 @@
         <v>524</v>
       </c>
       <c r="D51" s="156" t="s">
-        <v>539</v>
+        <v>556</v>
       </c>
       <c r="E51" s="150" t="s">
         <v>526</v>
@@ -17627,7 +17643,7 @@
         <v>527</v>
       </c>
       <c r="G51" s="153" t="s">
-        <v>555</v>
+        <v>557</v>
       </c>
       <c r="H51" s="15" t="s">
         <v>12</v>
@@ -17638,69 +17654,69 @@
       <c r="J51" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="153"/>
-      <c r="P51" s="153"/>
-      <c r="Q51" s="153"/>
-      <c r="R51" s="153"/>
-      <c r="S51" s="153"/>
-      <c r="T51" s="153"/>
-      <c r="U51" s="153"/>
-      <c r="V51" s="153"/>
-      <c r="W51" s="153"/>
-      <c r="X51" s="153"/>
-      <c r="Y51" s="153"/>
-      <c r="Z51" s="153"/>
     </row>
     <row r="52" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A52" s="151">
-        <v>204</v>
-      </c>
-      <c r="B52" s="15"/>
-      <c r="C52" s="156" t="s">
-        <v>524</v>
-      </c>
-      <c r="D52" s="156" t="s">
-        <v>556</v>
-      </c>
-      <c r="E52" s="150" t="s">
-        <v>526</v>
-      </c>
-      <c r="F52" s="153" t="s">
+      <c r="C52" s="146"/>
+    </row>
+    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A53" s="126"/>
+      <c r="B53" s="126"/>
+      <c r="C53" s="154" t="s">
+        <v>540</v>
+      </c>
+      <c r="D53" s="123"/>
+      <c r="E53" s="123"/>
+      <c r="F53" s="123"/>
+      <c r="G53" s="123"/>
+      <c r="H53" s="155"/>
+      <c r="I53" s="123"/>
+      <c r="J53" s="123"/>
+      <c r="K53" s="15"/>
+      <c r="L53" s="15"/>
+      <c r="M53" s="15"/>
+      <c r="N53" s="15"/>
+      <c r="O53" s="153"/>
+      <c r="P53" s="153"/>
+      <c r="Q53" s="153"/>
+      <c r="R53" s="153"/>
+      <c r="S53" s="153"/>
+      <c r="T53" s="153"/>
+      <c r="U53" s="153"/>
+      <c r="V53" s="153"/>
+      <c r="W53" s="153"/>
+      <c r="X53" s="153"/>
+      <c r="Y53" s="153"/>
+      <c r="Z53" s="153"/>
+    </row>
+    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A54" s="151">
+        <v>205</v>
+      </c>
+      <c r="B54" s="15"/>
+      <c r="C54" s="152" t="s">
+        <v>513</v>
+      </c>
+      <c r="D54" s="150" t="s">
+        <v>514</v>
+      </c>
+      <c r="E54" s="15" t="s">
+        <v>542</v>
+      </c>
+      <c r="F54" s="153" t="s">
         <v>527</v>
       </c>
-      <c r="G52" s="153" t="s">
-        <v>557</v>
-      </c>
-      <c r="H52" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I52" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J52" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="53" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C53" s="146"/>
-    </row>
-    <row r="54" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A54" s="126"/>
-      <c r="B54" s="126"/>
-      <c r="C54" s="154" t="s">
-        <v>540</v>
-      </c>
-      <c r="D54" s="123"/>
-      <c r="E54" s="123"/>
-      <c r="F54" s="123"/>
-      <c r="G54" s="123"/>
-      <c r="H54" s="155"/>
-      <c r="I54" s="123"/>
-      <c r="J54" s="123"/>
+      <c r="G54" s="153" t="s">
+        <v>516</v>
+      </c>
+      <c r="H54" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="I54" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="J54" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="K54" s="15"/>
       <c r="L54" s="15"/>
       <c r="M54" s="15"/>
@@ -17722,20 +17738,22 @@
       <c r="A55" s="151">
         <v>205</v>
       </c>
-      <c r="B55" s="126"/>
-      <c r="C55" s="178" t="s">
-        <v>562</v>
-      </c>
-      <c r="D55" s="179" t="s">
-        <v>562</v>
+      <c r="B55" s="15"/>
+      <c r="C55" s="152" t="s">
+        <v>517</v>
+      </c>
+      <c r="D55" s="150" t="s">
+        <v>514</v>
       </c>
       <c r="E55" s="15" t="s">
-        <v>563</v>
+        <v>542</v>
       </c>
       <c r="F55" s="153" t="s">
         <v>527</v>
       </c>
-      <c r="G55" s="15"/>
+      <c r="G55" s="153" t="s">
+        <v>518</v>
+      </c>
       <c r="H55" s="15" t="s">
         <v>12</v>
       </c>
@@ -17768,7 +17786,7 @@
       </c>
       <c r="B56" s="15"/>
       <c r="C56" s="152" t="s">
-        <v>513</v>
+        <v>519</v>
       </c>
       <c r="D56" s="150" t="s">
         <v>514</v>
@@ -17780,7 +17798,7 @@
         <v>527</v>
       </c>
       <c r="G56" s="153" t="s">
-        <v>516</v>
+        <v>520</v>
       </c>
       <c r="H56" s="15" t="s">
         <v>12</v>
@@ -17814,7 +17832,7 @@
       </c>
       <c r="B57" s="15"/>
       <c r="C57" s="152" t="s">
-        <v>517</v>
+        <v>521</v>
       </c>
       <c r="D57" s="150" t="s">
         <v>514</v>
@@ -17826,7 +17844,7 @@
         <v>527</v>
       </c>
       <c r="G57" s="153" t="s">
-        <v>518</v>
+        <v>522</v>
       </c>
       <c r="H57" s="15" t="s">
         <v>12</v>
@@ -17837,101 +17855,9 @@
       <c r="J57" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="153"/>
-      <c r="P57" s="153"/>
-      <c r="Q57" s="153"/>
-      <c r="R57" s="153"/>
-      <c r="S57" s="153"/>
-      <c r="T57" s="153"/>
-      <c r="U57" s="153"/>
-      <c r="V57" s="153"/>
-      <c r="W57" s="153"/>
-      <c r="X57" s="153"/>
-      <c r="Y57" s="153"/>
-      <c r="Z57" s="153"/>
-    </row>
-    <row r="58" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A58" s="151">
-        <v>205</v>
-      </c>
-      <c r="B58" s="15"/>
-      <c r="C58" s="152" t="s">
-        <v>519</v>
-      </c>
-      <c r="D58" s="150" t="s">
-        <v>514</v>
-      </c>
-      <c r="E58" s="15" t="s">
-        <v>542</v>
-      </c>
-      <c r="F58" s="153" t="s">
-        <v>527</v>
-      </c>
-      <c r="G58" s="153" t="s">
-        <v>520</v>
-      </c>
-      <c r="H58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I58" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J58" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="K58" s="15"/>
-      <c r="L58" s="15"/>
-      <c r="M58" s="15"/>
-      <c r="N58" s="15"/>
-      <c r="O58" s="153"/>
-      <c r="P58" s="153"/>
-      <c r="Q58" s="153"/>
-      <c r="R58" s="153"/>
-      <c r="S58" s="153"/>
-      <c r="T58" s="153"/>
-      <c r="U58" s="153"/>
-      <c r="V58" s="153"/>
-      <c r="W58" s="153"/>
-      <c r="X58" s="153"/>
-      <c r="Y58" s="153"/>
-      <c r="Z58" s="153"/>
     </row>
     <row r="59" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A59" s="151">
-        <v>205</v>
-      </c>
-      <c r="B59" s="15"/>
-      <c r="C59" s="152" t="s">
-        <v>521</v>
-      </c>
-      <c r="D59" s="150" t="s">
-        <v>514</v>
-      </c>
-      <c r="E59" s="15" t="s">
-        <v>542</v>
-      </c>
-      <c r="F59" s="153" t="s">
-        <v>527</v>
-      </c>
-      <c r="G59" s="153" t="s">
-        <v>522</v>
-      </c>
-      <c r="H59" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="I59" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="J59" s="15" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="61" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="C61" s="146"/>
+      <c r="C59" s="146"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
FRAT 15 TC 28.06.2019
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asif/Documents/AMT-TestFrameWork/src/main/resources/modules/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEDED0FA-7DE8-4741-8DE5-10050BB6EFE5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74842FE-0710-DE4C-BC45-F8636070A3D7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-2660" yWindow="-21600" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3371" uniqueCount="560">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3373" uniqueCount="561">
   <si>
     <t>Action</t>
   </si>
@@ -1717,6 +1717,9 @@
   </si>
   <si>
     <t>Test Common Step for 119</t>
+  </si>
+  <si>
+    <t>Check Duplicacy In LessorScheduleTable</t>
   </si>
 </sst>
 </file>
@@ -2463,30 +2466,6 @@
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2501,6 +2480,30 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -3189,7 +3192,7 @@
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="C25" sqref="C25"/>
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3566,7 +3569,13 @@
         <v>205</v>
       </c>
       <c r="C22" s="154" t="s">
-        <v>536</v>
+        <v>560</v>
+      </c>
+      <c r="D22" s="122" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" s="122" t="s">
+        <v>468</v>
       </c>
     </row>
   </sheetData>
@@ -3579,8 +3588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:L389"/>
   <sheetViews>
-    <sheetView topLeftCell="A193" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="E213" sqref="E213"/>
+    <sheetView topLeftCell="A328" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3637,16 +3646,16 @@
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="31"/>
       <c r="B2" s="32"/>
-      <c r="C2" s="174" t="s">
+      <c r="C2" s="179" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="174"/>
-      <c r="E2" s="174"/>
-      <c r="F2" s="174"/>
-      <c r="G2" s="174"/>
-      <c r="H2" s="174"/>
-      <c r="I2" s="174"/>
-      <c r="J2" s="174"/>
+      <c r="D2" s="179"/>
+      <c r="E2" s="179"/>
+      <c r="F2" s="179"/>
+      <c r="G2" s="179"/>
+      <c r="H2" s="179"/>
+      <c r="I2" s="179"/>
+      <c r="J2" s="179"/>
       <c r="K2" s="32"/>
       <c r="L2" s="33"/>
     </row>
@@ -4789,16 +4798,16 @@
     <row r="39" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A39" s="31"/>
       <c r="B39" s="32"/>
-      <c r="C39" s="174" t="s">
+      <c r="C39" s="179" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="174"/>
-      <c r="E39" s="174"/>
-      <c r="F39" s="174"/>
-      <c r="G39" s="174"/>
-      <c r="H39" s="174"/>
-      <c r="I39" s="174"/>
-      <c r="J39" s="174"/>
+      <c r="D39" s="179"/>
+      <c r="E39" s="179"/>
+      <c r="F39" s="179"/>
+      <c r="G39" s="179"/>
+      <c r="H39" s="179"/>
+      <c r="I39" s="179"/>
+      <c r="J39" s="179"/>
       <c r="K39" s="32"/>
       <c r="L39" s="33"/>
     </row>
@@ -6032,16 +6041,16 @@
     <row r="79" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A79" s="31"/>
       <c r="B79" s="32"/>
-      <c r="C79" s="174" t="s">
+      <c r="C79" s="179" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="174"/>
-      <c r="E79" s="174"/>
-      <c r="F79" s="174"/>
-      <c r="G79" s="174"/>
-      <c r="H79" s="174"/>
-      <c r="I79" s="174"/>
-      <c r="J79" s="174"/>
+      <c r="D79" s="179"/>
+      <c r="E79" s="179"/>
+      <c r="F79" s="179"/>
+      <c r="G79" s="179"/>
+      <c r="H79" s="179"/>
+      <c r="I79" s="179"/>
+      <c r="J79" s="179"/>
       <c r="K79" s="32"/>
       <c r="L79" s="33"/>
     </row>
@@ -7432,16 +7441,16 @@
     <row r="126" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A126" s="31"/>
       <c r="B126" s="32"/>
-      <c r="C126" s="174" t="s">
+      <c r="C126" s="179" t="s">
         <v>198</v>
       </c>
-      <c r="D126" s="174"/>
-      <c r="E126" s="174"/>
-      <c r="F126" s="174"/>
-      <c r="G126" s="174"/>
-      <c r="H126" s="174"/>
-      <c r="I126" s="174"/>
-      <c r="J126" s="174"/>
+      <c r="D126" s="179"/>
+      <c r="E126" s="179"/>
+      <c r="F126" s="179"/>
+      <c r="G126" s="179"/>
+      <c r="H126" s="179"/>
+      <c r="I126" s="179"/>
+      <c r="J126" s="179"/>
       <c r="K126" s="32"/>
       <c r="L126" s="33"/>
     </row>
@@ -8783,11 +8792,11 @@
       </c>
     </row>
     <row r="170" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B170" s="175" t="s">
+      <c r="B170" s="180" t="s">
         <v>206</v>
       </c>
-      <c r="C170" s="175"/>
-      <c r="D170" s="175"/>
+      <c r="C170" s="180"/>
+      <c r="D170" s="180"/>
       <c r="H170" s="75"/>
     </row>
     <row r="171" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -9296,11 +9305,11 @@
       <c r="J186" s="18"/>
     </row>
     <row r="187" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B187" s="170" t="s">
+      <c r="B187" s="177" t="s">
         <v>211</v>
       </c>
-      <c r="C187" s="170"/>
-      <c r="D187" s="170"/>
+      <c r="C187" s="177"/>
+      <c r="D187" s="177"/>
       <c r="H187" s="83"/>
     </row>
     <row r="188" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -9619,11 +9628,11 @@
       </c>
     </row>
     <row r="201" spans="1:12" s="87" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B201" s="171" t="s">
+      <c r="B201" s="181" t="s">
         <v>202</v>
       </c>
-      <c r="C201" s="171"/>
-      <c r="D201" s="171"/>
+      <c r="C201" s="181"/>
+      <c r="D201" s="181"/>
       <c r="H201" s="88"/>
     </row>
     <row r="202" spans="1:12" s="110" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -10179,11 +10188,11 @@
       </c>
     </row>
     <row r="220" spans="1:12" s="74" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B220" s="172" t="s">
+      <c r="B220" s="182" t="s">
         <v>203</v>
       </c>
-      <c r="C220" s="172"/>
-      <c r="D220" s="172"/>
+      <c r="C220" s="182"/>
+      <c r="D220" s="182"/>
       <c r="H220" s="75"/>
     </row>
     <row r="221" spans="1:12" s="95" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -11240,11 +11249,11 @@
       </c>
     </row>
     <row r="254" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B254" s="173" t="s">
+      <c r="B254" s="183" t="s">
         <v>204</v>
       </c>
-      <c r="C254" s="173"/>
-      <c r="D254" s="173"/>
+      <c r="C254" s="183"/>
+      <c r="D254" s="183"/>
       <c r="H254" s="83"/>
     </row>
     <row r="255" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -11622,11 +11631,11 @@
       </c>
     </row>
     <row r="267" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B267" s="173" t="s">
+      <c r="B267" s="183" t="s">
         <v>205</v>
       </c>
-      <c r="C267" s="173"/>
-      <c r="D267" s="173"/>
+      <c r="C267" s="183"/>
+      <c r="D267" s="183"/>
       <c r="H267" s="83"/>
     </row>
     <row r="268" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -12342,11 +12351,11 @@
       </c>
     </row>
     <row r="291" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B291" s="170" t="s">
+      <c r="B291" s="177" t="s">
         <v>415</v>
       </c>
-      <c r="C291" s="170"/>
-      <c r="D291" s="170"/>
+      <c r="C291" s="177"/>
+      <c r="D291" s="177"/>
       <c r="H291" s="83"/>
     </row>
     <row r="292" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -12646,11 +12655,11 @@
       </c>
     </row>
     <row r="301" spans="1:12" s="82" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="B301" s="177" t="s">
+      <c r="B301" s="178" t="s">
         <v>414</v>
       </c>
-      <c r="C301" s="177"/>
-      <c r="D301" s="177"/>
+      <c r="C301" s="178"/>
+      <c r="D301" s="178"/>
       <c r="H301" s="83"/>
     </row>
     <row r="302" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -15370,6 +15379,16 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B187:D187"/>
+    <mergeCell ref="B201:D201"/>
+    <mergeCell ref="B220:D220"/>
+    <mergeCell ref="B254:D254"/>
+    <mergeCell ref="B267:D267"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C126:J126"/>
+    <mergeCell ref="B170:D170"/>
     <mergeCell ref="B360:E360"/>
     <mergeCell ref="B291:D291"/>
     <mergeCell ref="B301:D301"/>
@@ -15377,16 +15396,6 @@
     <mergeCell ref="B383:E383"/>
     <mergeCell ref="B310:E310"/>
     <mergeCell ref="B328:E328"/>
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C126:J126"/>
-    <mergeCell ref="B170:D170"/>
-    <mergeCell ref="B187:D187"/>
-    <mergeCell ref="B201:D201"/>
-    <mergeCell ref="B220:D220"/>
-    <mergeCell ref="B254:D254"/>
-    <mergeCell ref="B267:D267"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="43" priority="425" operator="equal">
@@ -15889,8 +15898,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{67A52F28-3949-0E4C-AC35-967E0AD937B0}">
   <dimension ref="A1:Z73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -16354,7 +16363,7 @@
     </row>
     <row r="16" spans="1:12" s="123" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A16" s="126"/>
-      <c r="C16" s="182" t="s">
+      <c r="C16" s="174" t="s">
         <v>559</v>
       </c>
       <c r="H16" s="126"/>
@@ -16822,7 +16831,7 @@
     </row>
     <row r="31" spans="1:16" s="123" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A31" s="126"/>
-      <c r="C31" s="182" t="s">
+      <c r="C31" s="174" t="s">
         <v>469</v>
       </c>
       <c r="H31" s="126"/>
@@ -17136,33 +17145,33 @@
       <c r="A40" s="162">
         <v>119</v>
       </c>
-      <c r="B40" s="178"/>
-      <c r="C40" s="179" t="s">
+      <c r="B40" s="170"/>
+      <c r="C40" s="171" t="s">
         <v>504</v>
       </c>
-      <c r="D40" s="179" t="s">
+      <c r="D40" s="171" t="s">
         <v>505</v>
       </c>
-      <c r="E40" s="183" t="s">
+      <c r="E40" s="175" t="s">
         <v>416</v>
       </c>
       <c r="F40" s="136" t="s">
         <v>508</v>
       </c>
-      <c r="G40" s="179" t="s">
+      <c r="G40" s="171" t="s">
         <v>151</v>
       </c>
-      <c r="H40" s="181" t="s">
-        <v>12</v>
-      </c>
-      <c r="I40" s="178" t="s">
-        <v>2</v>
-      </c>
-      <c r="J40" s="181" t="s">
+      <c r="H40" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="170" t="s">
+        <v>2</v>
+      </c>
+      <c r="J40" s="173" t="s">
         <v>12</v>
       </c>
       <c r="K40" s="137"/>
-      <c r="L40" s="181">
+      <c r="L40" s="173">
         <v>0</v>
       </c>
       <c r="M40" s="137"/>
@@ -17171,87 +17180,83 @@
       <c r="P40" s="137"/>
     </row>
     <row r="41" spans="1:26" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="162">
-        <v>119</v>
-      </c>
-      <c r="B41" s="178"/>
-      <c r="C41" s="179" t="s">
+      <c r="A41" s="162"/>
+      <c r="B41" s="170"/>
+      <c r="C41" s="171" t="s">
         <v>554</v>
       </c>
-      <c r="D41" s="179" t="s">
+      <c r="D41" s="171" t="s">
         <v>539</v>
       </c>
-      <c r="E41" s="180" t="s">
+      <c r="E41" s="172" t="s">
         <v>439</v>
       </c>
       <c r="F41" s="136" t="s">
         <v>555</v>
       </c>
-      <c r="H41" s="181" t="s">
-        <v>12</v>
-      </c>
-      <c r="I41" s="178" t="s">
-        <v>2</v>
-      </c>
-      <c r="J41" s="181" t="s">
+      <c r="H41" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="I41" s="170" t="s">
+        <v>2</v>
+      </c>
+      <c r="J41" s="173" t="s">
         <v>12</v>
       </c>
       <c r="K41" s="137"/>
-      <c r="L41" s="181">
+      <c r="L41" s="173">
         <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:26" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="162">
-        <v>119</v>
-      </c>
-      <c r="B42" s="178"/>
-      <c r="C42" s="179" t="s">
+      <c r="A42" s="162"/>
+      <c r="B42" s="170"/>
+      <c r="C42" s="171" t="s">
         <v>554</v>
       </c>
-      <c r="D42" s="179" t="s">
+      <c r="D42" s="171" t="s">
         <v>539</v>
       </c>
-      <c r="E42" s="180" t="s">
+      <c r="E42" s="172" t="s">
         <v>558</v>
       </c>
       <c r="F42" s="136" t="s">
         <v>555</v>
       </c>
-      <c r="H42" s="181" t="s">
-        <v>12</v>
-      </c>
-      <c r="I42" s="178" t="s">
-        <v>2</v>
-      </c>
-      <c r="J42" s="181" t="s">
-        <v>12</v>
-      </c>
-      <c r="L42" s="181">
+      <c r="H42" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="I42" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="J42" s="173" t="s">
+        <v>12</v>
+      </c>
+      <c r="L42" s="173">
         <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:26" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="181"/>
-      <c r="B43" s="178"/>
-      <c r="C43" s="179"/>
-      <c r="D43" s="179"/>
-      <c r="E43" s="180"/>
-      <c r="H43" s="181"/>
-      <c r="I43" s="178"/>
-      <c r="J43" s="181"/>
-      <c r="L43" s="181"/>
+      <c r="A43" s="173"/>
+      <c r="B43" s="170"/>
+      <c r="C43" s="171"/>
+      <c r="D43" s="171"/>
+      <c r="E43" s="150"/>
+      <c r="H43" s="173"/>
+      <c r="I43" s="170"/>
+      <c r="J43" s="173"/>
+      <c r="L43" s="173"/>
     </row>
     <row r="44" spans="1:26" s="136" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="181"/>
-      <c r="B44" s="178"/>
-      <c r="C44" s="179"/>
-      <c r="D44" s="179"/>
-      <c r="E44" s="180"/>
-      <c r="H44" s="181"/>
-      <c r="I44" s="178"/>
-      <c r="J44" s="181"/>
-      <c r="L44" s="181"/>
+      <c r="A44" s="173"/>
+      <c r="B44" s="170"/>
+      <c r="C44" s="171"/>
+      <c r="D44" s="171"/>
+      <c r="E44" s="172"/>
+      <c r="H44" s="173"/>
+      <c r="I44" s="170"/>
+      <c r="J44" s="173"/>
+      <c r="L44" s="173"/>
     </row>
     <row r="45" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A45" s="162"/>

</xml_diff>

<commit_message>
Release the smoke test cases
</commit_message>
<xml_diff>
--- a/src/main/resources/modules/CommonTC.xlsx
+++ b/src/main/resources/modules/CommonTC.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2715" windowWidth="32715" windowHeight="20535" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="4065" windowWidth="32715" windowHeight="20535" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Controller" sheetId="19" r:id="rId1"/>
@@ -4243,6 +4243,9 @@
     <xf numFmtId="0" fontId="4" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -4262,9 +4265,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -4450,25 +4450,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4614,25 +4597,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4771,25 +4737,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -4921,25 +4870,8 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
+        <patternFill>
+          <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5071,30 +5003,6 @@
     </dxf>
     <dxf>
       <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
@@ -5188,58 +5096,6 @@
       <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFED7D31"/>
-          <bgColor rgb="FFED7D31"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF4B083"/>
-          <bgColor rgb="FFF4B083"/>
         </patternFill>
       </fill>
     </dxf>
@@ -7775,6 +7631,150 @@
     </dxf>
     <dxf>
       <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFED7D31"/>
+          <bgColor rgb="FFED7D31"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF4B083"/>
+          <bgColor rgb="FFF4B083"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
         <patternFill>
           <bgColor theme="5" tint="0.39994506668294322"/>
         </patternFill>
@@ -9715,8 +9715,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:XFD451"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A183" sqref="A183:XFD183"/>
+    <sheetView tabSelected="1" topLeftCell="C226" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I230" sqref="I230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
@@ -9774,16 +9774,16 @@
     <row r="2" spans="1:12">
       <c r="A2" s="29"/>
       <c r="B2" s="30"/>
-      <c r="C2" s="374" t="s">
+      <c r="C2" s="367" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="374"/>
-      <c r="E2" s="374"/>
-      <c r="F2" s="374"/>
-      <c r="G2" s="374"/>
-      <c r="H2" s="374"/>
-      <c r="I2" s="374"/>
-      <c r="J2" s="374"/>
+      <c r="D2" s="367"/>
+      <c r="E2" s="367"/>
+      <c r="F2" s="367"/>
+      <c r="G2" s="367"/>
+      <c r="H2" s="367"/>
+      <c r="I2" s="367"/>
+      <c r="J2" s="367"/>
       <c r="K2" s="30"/>
       <c r="L2" s="31"/>
     </row>
@@ -10923,16 +10923,16 @@
     <row r="39" spans="1:12">
       <c r="A39" s="29"/>
       <c r="B39" s="30"/>
-      <c r="C39" s="374" t="s">
+      <c r="C39" s="367" t="s">
         <v>159</v>
       </c>
-      <c r="D39" s="374"/>
-      <c r="E39" s="374"/>
-      <c r="F39" s="374"/>
-      <c r="G39" s="374"/>
-      <c r="H39" s="374"/>
-      <c r="I39" s="374"/>
-      <c r="J39" s="374"/>
+      <c r="D39" s="367"/>
+      <c r="E39" s="367"/>
+      <c r="F39" s="367"/>
+      <c r="G39" s="367"/>
+      <c r="H39" s="367"/>
+      <c r="I39" s="367"/>
+      <c r="J39" s="367"/>
       <c r="K39" s="30"/>
       <c r="L39" s="31"/>
     </row>
@@ -12165,16 +12165,16 @@
     <row r="79" spans="1:12">
       <c r="A79" s="29"/>
       <c r="B79" s="30"/>
-      <c r="C79" s="374" t="s">
+      <c r="C79" s="367" t="s">
         <v>190</v>
       </c>
-      <c r="D79" s="374"/>
-      <c r="E79" s="374"/>
-      <c r="F79" s="374"/>
-      <c r="G79" s="374"/>
-      <c r="H79" s="374"/>
-      <c r="I79" s="374"/>
-      <c r="J79" s="374"/>
+      <c r="D79" s="367"/>
+      <c r="E79" s="367"/>
+      <c r="F79" s="367"/>
+      <c r="G79" s="367"/>
+      <c r="H79" s="367"/>
+      <c r="I79" s="367"/>
+      <c r="J79" s="367"/>
       <c r="K79" s="30"/>
       <c r="L79" s="31"/>
     </row>
@@ -13561,16 +13561,16 @@
     <row r="126" spans="1:12">
       <c r="A126" s="29"/>
       <c r="B126" s="30"/>
-      <c r="C126" s="374" t="s">
+      <c r="C126" s="367" t="s">
         <v>198</v>
       </c>
-      <c r="D126" s="374"/>
-      <c r="E126" s="374"/>
-      <c r="F126" s="374"/>
-      <c r="G126" s="374"/>
-      <c r="H126" s="374"/>
-      <c r="I126" s="374"/>
-      <c r="J126" s="374"/>
+      <c r="D126" s="367"/>
+      <c r="E126" s="367"/>
+      <c r="F126" s="367"/>
+      <c r="G126" s="367"/>
+      <c r="H126" s="367"/>
+      <c r="I126" s="367"/>
+      <c r="J126" s="367"/>
       <c r="K126" s="30"/>
       <c r="L126" s="31"/>
     </row>
@@ -14913,11 +14913,11 @@
     </row>
     <row r="170" spans="1:16384" s="71" customFormat="1">
       <c r="A170" s="116"/>
-      <c r="B170" s="367" t="s">
+      <c r="B170" s="368" t="s">
         <v>206</v>
       </c>
-      <c r="C170" s="367"/>
-      <c r="D170" s="367"/>
+      <c r="C170" s="368"/>
+      <c r="D170" s="368"/>
       <c r="H170" s="141"/>
       <c r="I170" s="121"/>
       <c r="J170" s="121"/>
@@ -31838,11 +31838,11 @@
     </row>
     <row r="188" spans="1:12" s="78" customFormat="1">
       <c r="A188" s="123"/>
-      <c r="B188" s="368" t="s">
+      <c r="B188" s="369" t="s">
         <v>211</v>
       </c>
-      <c r="C188" s="368"/>
-      <c r="D188" s="368"/>
+      <c r="C188" s="369"/>
+      <c r="D188" s="369"/>
       <c r="H188" s="142"/>
       <c r="I188" s="123"/>
       <c r="J188" s="123"/>
@@ -32164,11 +32164,11 @@
     </row>
     <row r="202" spans="1:12" s="82" customFormat="1">
       <c r="A202" s="124"/>
-      <c r="B202" s="369" t="s">
+      <c r="B202" s="370" t="s">
         <v>202</v>
       </c>
-      <c r="C202" s="369"/>
-      <c r="D202" s="369"/>
+      <c r="C202" s="370"/>
+      <c r="D202" s="370"/>
       <c r="H202" s="143"/>
       <c r="I202" s="124"/>
       <c r="J202" s="124"/>
@@ -32728,11 +32728,11 @@
     </row>
     <row r="221" spans="1:12" s="71" customFormat="1">
       <c r="A221" s="116"/>
-      <c r="B221" s="370" t="s">
+      <c r="B221" s="371" t="s">
         <v>203</v>
       </c>
-      <c r="C221" s="370"/>
-      <c r="D221" s="370"/>
+      <c r="C221" s="371"/>
+      <c r="D221" s="371"/>
       <c r="H221" s="141"/>
       <c r="I221" s="121"/>
       <c r="J221" s="121"/>
@@ -33015,7 +33015,7 @@
         <v>12</v>
       </c>
       <c r="I230" s="90" t="s">
-        <v>2</v>
+        <v>12</v>
       </c>
       <c r="J230" s="94" t="s">
         <v>12</v>
@@ -33792,11 +33792,11 @@
     </row>
     <row r="255" spans="1:12" s="78" customFormat="1">
       <c r="A255" s="123"/>
-      <c r="B255" s="371" t="s">
+      <c r="B255" s="372" t="s">
         <v>204</v>
       </c>
-      <c r="C255" s="371"/>
-      <c r="D255" s="371"/>
+      <c r="C255" s="372"/>
+      <c r="D255" s="372"/>
       <c r="H255" s="142"/>
       <c r="I255" s="123"/>
       <c r="J255" s="123"/>
@@ -34180,11 +34180,11 @@
     </row>
     <row r="268" spans="1:12" s="78" customFormat="1">
       <c r="A268" s="123"/>
-      <c r="B268" s="371" t="s">
+      <c r="B268" s="372" t="s">
         <v>205</v>
       </c>
-      <c r="C268" s="371"/>
-      <c r="D268" s="371"/>
+      <c r="C268" s="372"/>
+      <c r="D268" s="372"/>
       <c r="H268" s="142"/>
       <c r="I268" s="123"/>
       <c r="J268" s="123"/>
@@ -34903,11 +34903,11 @@
     </row>
     <row r="292" spans="1:12" s="78" customFormat="1">
       <c r="A292" s="123"/>
-      <c r="B292" s="368" t="s">
+      <c r="B292" s="369" t="s">
         <v>414</v>
       </c>
-      <c r="C292" s="368"/>
-      <c r="D292" s="368"/>
+      <c r="C292" s="369"/>
+      <c r="D292" s="369"/>
       <c r="H292" s="142"/>
       <c r="I292" s="123"/>
       <c r="J292" s="123"/>
@@ -35223,11 +35223,11 @@
     </row>
     <row r="303" spans="1:12" s="78" customFormat="1">
       <c r="A303" s="123"/>
-      <c r="B303" s="373" t="s">
+      <c r="B303" s="374" t="s">
         <v>413</v>
       </c>
-      <c r="C303" s="373"/>
-      <c r="D303" s="373"/>
+      <c r="C303" s="374"/>
+      <c r="D303" s="374"/>
       <c r="H303" s="142"/>
       <c r="I303" s="123"/>
       <c r="J303" s="123"/>
@@ -35509,12 +35509,12 @@
     </row>
     <row r="313" spans="1:12">
       <c r="A313" s="115"/>
-      <c r="B313" s="372" t="s">
+      <c r="B313" s="373" t="s">
         <v>423</v>
       </c>
-      <c r="C313" s="372"/>
-      <c r="D313" s="372"/>
-      <c r="E313" s="372"/>
+      <c r="C313" s="373"/>
+      <c r="D313" s="373"/>
+      <c r="E313" s="373"/>
       <c r="F313" s="105"/>
       <c r="G313" s="105"/>
       <c r="H313" s="144"/>
@@ -35909,12 +35909,12 @@
     </row>
     <row r="327" spans="1:12">
       <c r="A327" s="115"/>
-      <c r="B327" s="372" t="s">
+      <c r="B327" s="373" t="s">
         <v>430</v>
       </c>
-      <c r="C327" s="372"/>
-      <c r="D327" s="372"/>
-      <c r="E327" s="372"/>
+      <c r="C327" s="373"/>
+      <c r="D327" s="373"/>
+      <c r="E327" s="373"/>
       <c r="F327" s="105"/>
       <c r="G327" s="105"/>
       <c r="H327" s="144"/>
@@ -36915,12 +36915,12 @@
     </row>
     <row r="359" spans="1:12">
       <c r="A359" s="115"/>
-      <c r="B359" s="372" t="s">
+      <c r="B359" s="373" t="s">
         <v>432</v>
       </c>
-      <c r="C359" s="372"/>
-      <c r="D359" s="372"/>
-      <c r="E359" s="372"/>
+      <c r="C359" s="373"/>
+      <c r="D359" s="373"/>
+      <c r="E359" s="373"/>
       <c r="F359" s="105"/>
       <c r="G359" s="105"/>
       <c r="H359" s="144"/>
@@ -37242,8 +37242,8 @@
       <c r="H368" s="144" t="s">
         <v>12</v>
       </c>
-      <c r="I368" s="17" t="s">
-        <v>2</v>
+      <c r="I368" s="26" t="s">
+        <v>12</v>
       </c>
       <c r="J368" s="44" t="s">
         <v>12</v>
@@ -37442,12 +37442,12 @@
     </row>
     <row r="375" spans="1:26">
       <c r="A375" s="115"/>
-      <c r="B375" s="372" t="s">
+      <c r="B375" s="373" t="s">
         <v>451</v>
       </c>
-      <c r="C375" s="372"/>
-      <c r="D375" s="372"/>
-      <c r="E375" s="372"/>
+      <c r="C375" s="373"/>
+      <c r="D375" s="373"/>
+      <c r="E375" s="373"/>
       <c r="F375" s="105"/>
       <c r="G375" s="105"/>
       <c r="H375" s="144"/>
@@ -37676,12 +37676,12 @@
     </row>
     <row r="384" spans="1:26">
       <c r="A384" s="115"/>
-      <c r="B384" s="372" t="s">
+      <c r="B384" s="373" t="s">
         <v>452</v>
       </c>
-      <c r="C384" s="372"/>
-      <c r="D384" s="372"/>
-      <c r="E384" s="372"/>
+      <c r="C384" s="373"/>
+      <c r="D384" s="373"/>
+      <c r="E384" s="373"/>
       <c r="F384" s="105"/>
       <c r="G384" s="105"/>
       <c r="H384" s="144"/>
@@ -38177,11 +38177,11 @@
     </row>
     <row r="403" spans="1:12" s="71" customFormat="1">
       <c r="A403" s="116"/>
-      <c r="B403" s="367" t="s">
+      <c r="B403" s="368" t="s">
         <v>462</v>
       </c>
-      <c r="C403" s="367"/>
-      <c r="D403" s="367"/>
+      <c r="C403" s="368"/>
+      <c r="D403" s="368"/>
       <c r="H403" s="141"/>
       <c r="I403" s="121"/>
       <c r="J403" s="121"/>
@@ -38466,7 +38466,7 @@
         <v>2</v>
       </c>
       <c r="J412" s="35" t="s">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="K412" s="36" t="s">
         <v>468</v>
@@ -39598,11 +39598,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C2:J2"/>
-    <mergeCell ref="C39:J39"/>
-    <mergeCell ref="C79:J79"/>
-    <mergeCell ref="C126:J126"/>
-    <mergeCell ref="B170:D170"/>
     <mergeCell ref="B403:D403"/>
     <mergeCell ref="B188:D188"/>
     <mergeCell ref="B202:D202"/>
@@ -39616,6 +39611,11 @@
     <mergeCell ref="B384:E384"/>
     <mergeCell ref="B313:E313"/>
     <mergeCell ref="B327:E327"/>
+    <mergeCell ref="C2:J2"/>
+    <mergeCell ref="C39:J39"/>
+    <mergeCell ref="C79:J79"/>
+    <mergeCell ref="C126:J126"/>
+    <mergeCell ref="B170:D170"/>
   </mergeCells>
   <conditionalFormatting sqref="H26">
     <cfRule type="cellIs" dxfId="547" priority="445" operator="equal">
@@ -40378,7 +40378,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z644"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D355" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="I387" sqref="I386:I387"/>
     </sheetView>
   </sheetViews>
@@ -57688,12 +57688,31 @@
     </row>
   </sheetData>
   <mergeCells count="47">
-    <mergeCell ref="C595:F595"/>
-    <mergeCell ref="C621:F621"/>
-    <mergeCell ref="C498:F498"/>
-    <mergeCell ref="C522:F522"/>
-    <mergeCell ref="C546:F546"/>
-    <mergeCell ref="C570:F570"/>
+    <mergeCell ref="C404:F404"/>
+    <mergeCell ref="C418:F418"/>
+    <mergeCell ref="C433:F433"/>
+    <mergeCell ref="C282:F282"/>
+    <mergeCell ref="C289:F289"/>
+    <mergeCell ref="C380:F380"/>
+    <mergeCell ref="C397:F397"/>
+    <mergeCell ref="C324:F324"/>
+    <mergeCell ref="C338:F338"/>
+    <mergeCell ref="C344:F344"/>
+    <mergeCell ref="C358:F358"/>
+    <mergeCell ref="C365:F365"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="C41:F41"/>
+    <mergeCell ref="C55:F55"/>
+    <mergeCell ref="C62:F62"/>
+    <mergeCell ref="C73:F73"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="C13:F13"/>
+    <mergeCell ref="C132:F132"/>
+    <mergeCell ref="C84:F84"/>
+    <mergeCell ref="C107:F107"/>
+    <mergeCell ref="C96:F96"/>
+    <mergeCell ref="C118:F118"/>
     <mergeCell ref="C440:F440"/>
     <mergeCell ref="C465:F465"/>
     <mergeCell ref="C491:F491"/>
@@ -57710,31 +57729,12 @@
     <mergeCell ref="C246:F246"/>
     <mergeCell ref="C260:F260"/>
     <mergeCell ref="C267:F267"/>
-    <mergeCell ref="C132:F132"/>
-    <mergeCell ref="C84:F84"/>
-    <mergeCell ref="C107:F107"/>
-    <mergeCell ref="C96:F96"/>
-    <mergeCell ref="C118:F118"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="C41:F41"/>
-    <mergeCell ref="C55:F55"/>
-    <mergeCell ref="C62:F62"/>
-    <mergeCell ref="C73:F73"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="C13:F13"/>
-    <mergeCell ref="C404:F404"/>
-    <mergeCell ref="C418:F418"/>
-    <mergeCell ref="C433:F433"/>
-    <mergeCell ref="C282:F282"/>
-    <mergeCell ref="C289:F289"/>
-    <mergeCell ref="C380:F380"/>
-    <mergeCell ref="C397:F397"/>
-    <mergeCell ref="C324:F324"/>
-    <mergeCell ref="C338:F338"/>
-    <mergeCell ref="C344:F344"/>
-    <mergeCell ref="C358:F358"/>
-    <mergeCell ref="C365:F365"/>
+    <mergeCell ref="C595:F595"/>
+    <mergeCell ref="C621:F621"/>
+    <mergeCell ref="C498:F498"/>
+    <mergeCell ref="C522:F522"/>
+    <mergeCell ref="C546:F546"/>
+    <mergeCell ref="C570:F570"/>
   </mergeCells>
   <conditionalFormatting sqref="H41">
     <cfRule type="cellIs" dxfId="486" priority="550" operator="equal">
@@ -57962,92 +57962,92 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H498">
-    <cfRule type="cellIs" dxfId="131" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="441" priority="157" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H498">
-    <cfRule type="cellIs" dxfId="130" priority="158" operator="equal">
+    <cfRule type="cellIs" dxfId="440" priority="158" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H498">
-    <cfRule type="cellIs" dxfId="129" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="439" priority="159" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H522">
-    <cfRule type="cellIs" dxfId="110" priority="109" operator="equal">
+    <cfRule type="cellIs" dxfId="438" priority="109" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H522">
-    <cfRule type="cellIs" dxfId="109" priority="110" operator="equal">
+    <cfRule type="cellIs" dxfId="437" priority="110" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H522">
-    <cfRule type="cellIs" dxfId="108" priority="111" operator="equal">
+    <cfRule type="cellIs" dxfId="436" priority="111" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H546">
-    <cfRule type="cellIs" dxfId="89" priority="88" operator="equal">
+    <cfRule type="cellIs" dxfId="435" priority="88" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H546">
-    <cfRule type="cellIs" dxfId="88" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="434" priority="89" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H546">
-    <cfRule type="cellIs" dxfId="87" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="433" priority="90" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H570">
-    <cfRule type="cellIs" dxfId="68" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="432" priority="67" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H570">
-    <cfRule type="cellIs" dxfId="67" priority="68" operator="equal">
+    <cfRule type="cellIs" dxfId="431" priority="68" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H570">
-    <cfRule type="cellIs" dxfId="66" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="430" priority="69" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H595">
-    <cfRule type="cellIs" dxfId="46" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="429" priority="45" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H595">
-    <cfRule type="cellIs" dxfId="45" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="428" priority="46" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H595">
-    <cfRule type="cellIs" dxfId="44" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="427" priority="47" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H621">
-    <cfRule type="cellIs" dxfId="23" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="426" priority="22" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H621">
-    <cfRule type="cellIs" dxfId="22" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="425" priority="23" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H621">
-    <cfRule type="cellIs" dxfId="21" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="424" priority="24" operator="equal">
       <formula>#REF!</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>